<commit_message>
release notes (1st draft) and a small update of the functors mapping
</commit_message>
<xml_diff>
--- a/tecto2umr/pdt-c-functors-to-args.xlsx
+++ b/tecto2umr/pdt-c-functors-to-args.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="19050" windowHeight="6705"/>
   </bookViews>
@@ -17,14 +12,14 @@
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$D$1:$D$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$E$1:$E$122</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="252">
   <si>
     <t>RSTR</t>
   </si>
@@ -944,21 +939,12 @@
     <t>refer-number</t>
   </si>
   <si>
-    <t>subrole … attribute of NE concepts (not relation)</t>
-  </si>
-  <si>
-    <t>subrole … attribute of quantity/quantity concepts (not relation)</t>
-  </si>
-  <si>
     <t>attribute of ?event node</t>
   </si>
   <si>
     <t>attribute of event node</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>attribute of entity  node</t>
   </si>
   <si>
@@ -981,9 +967,6 @@
   </si>
   <si>
     <t>subtraction</t>
-  </si>
-  <si>
-    <t>discurse role</t>
   </si>
   <si>
     <r>
@@ -1433,12 +1416,6 @@
     <t>contrast-91</t>
   </si>
   <si>
-    <t>discourse role</t>
-  </si>
-  <si>
-    <t>NON-part. role</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1666,24 +1643,6 @@
   </si>
   <si>
     <t xml:space="preserve">UMR rozlišuje date-interval, value-interval, between, slash </t>
-  </si>
-  <si>
-    <r>
-      <t>TODO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - hyperrole</t>
-    </r>
-  </si>
-  <si>
-    <t>event, args</t>
   </si>
   <si>
     <t>ARG1 for main clause, ARG2 for contrastive clause</t>
@@ -2440,12 +2399,182 @@
  </t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>TODO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - new abstract concept</t>
+    </r>
+  </si>
+  <si>
+    <t>… attribute of quantity/quantity concepts (not relation)</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attribute </t>
+  </si>
+  <si>
+    <t>role, participant</t>
+  </si>
+  <si>
+    <t>role, NON-participant</t>
+  </si>
+  <si>
+    <t>concept, event, args</t>
+  </si>
+  <si>
+    <t>concept, abstract entity; ops</t>
+  </si>
+  <si>
+    <t>role, discourse relation</t>
+  </si>
+  <si>
+    <t>subrole for NE concepts (not relation)</t>
+  </si>
+  <si>
+    <t>subrole, NE</t>
+  </si>
+  <si>
+    <t>subrole,quantity/quantity concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subrole, quantity/quantity concepts </t>
+  </si>
+  <si>
+    <t>subrole, date-entity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">intensifier , downtoner , or equal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>… 3-3-6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">include: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>imperative</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">expressive </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>interrogative</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(typically for main predicate) … </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3-3-2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2571,8 +2700,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2328"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F2328"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2328"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2594,18 +2743,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2648,9 +2785,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2713,67 +2850,52 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2815,11 +2937,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
+    <cellStyle name="Kontrolní buňka" xfId="2" builtinId="23"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2835,9 +2958,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kancelář">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2875,9 +2998,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2912,7 +3035,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2947,7 +3070,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kancelář">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3123,17 +3246,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="4"/>
     <col min="3" max="3" width="10" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="6" customWidth="1"/>
     <col min="6" max="6" width="62" style="15" customWidth="1"/>
     <col min="7" max="7" width="67.42578125" style="13" customWidth="1"/>
     <col min="8" max="8" width="44.140625" style="14" customWidth="1"/>
@@ -3141,39 +3264,39 @@
     <col min="10" max="10" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="33">
+    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="36">
+      <c r="H1" s="31">
         <v>2014</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="28" t="s">
         <v>100</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3184,10 +3307,10 @@
         <v>10207</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -3198,10 +3321,10 @@
         <v>8427</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -3212,10 +3335,10 @@
         <v>2793</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>0</v>
       </c>
@@ -3226,11 +3349,11 @@
         <v>209767</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>0</v>
       </c>
@@ -3241,23 +3364,23 @@
         <v>422</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="33">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28">
         <v>0</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" spans="1:10" ht="120.75" thickTop="1">
+      <c r="B7" s="30"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -3271,16 +3394,16 @@
         <v>72</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="165">
+    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -3294,16 +3417,16 @@
         <v>73</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>3</v>
       </c>
@@ -3317,7 +3440,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>122</v>
@@ -3326,7 +3449,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>4</v>
       </c>
@@ -3340,13 +3463,13 @@
         <v>84</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>112</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>79</v>
@@ -3355,7 +3478,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30.75" thickBot="1">
+    <row r="12" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>5</v>
       </c>
@@ -3369,10 +3492,10 @@
         <v>98</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>80</v>
@@ -3381,20 +3504,20 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A13" s="33">
+    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28">
         <v>6</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickTop="1">
+      <c r="B13" s="30"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>7</v>
       </c>
@@ -3414,7 +3537,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>8</v>
       </c>
@@ -3428,11 +3551,11 @@
         <v>83</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>9</v>
       </c>
@@ -3446,13 +3569,13 @@
         <v>82</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>10</v>
       </c>
@@ -3466,14 +3589,14 @@
         <v>83</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F17" s="2"/>
       <c r="H17" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>11</v>
       </c>
@@ -3487,11 +3610,11 @@
         <v>103</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>12</v>
       </c>
@@ -3505,7 +3628,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>13</v>
       </c>
@@ -3519,7 +3642,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>14</v>
       </c>
@@ -3533,7 +3656,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>15</v>
       </c>
@@ -3547,49 +3670,49 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A23" s="38">
+    <row r="23" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="33">
         <v>16</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-    </row>
-    <row r="24" spans="1:9" ht="75.75" thickTop="1">
-      <c r="A24" s="39">
+      <c r="B23" s="35"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+    </row>
+    <row r="24" spans="1:9" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34">
         <v>17</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="38">
         <v>17394</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="G24" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="H24" s="49" t="s">
+      <c r="E24" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="H24" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="50" t="s">
+      <c r="I24" s="45" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>18</v>
       </c>
@@ -3603,7 +3726,7 @@
         <v>105</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>110</v>
@@ -3615,7 +3738,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="60">
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>19</v>
       </c>
@@ -3629,7 +3752,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>111</v>
@@ -3641,7 +3764,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>20</v>
       </c>
@@ -3655,7 +3778,7 @@
         <v>67</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>113</v>
@@ -3667,37 +3790,37 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A28" s="38">
+    <row r="28" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="33">
         <v>21</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A29" s="39">
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="34">
         <v>22</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="46" t="s">
+      <c r="B29" s="36"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="G29" s="47"/>
-      <c r="H29" s="49" t="s">
+      <c r="G29" s="42"/>
+      <c r="H29" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="I29" s="49"/>
-    </row>
-    <row r="30" spans="1:9" ht="30">
+      <c r="I29" s="44"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>23</v>
       </c>
@@ -3711,7 +3834,7 @@
         <v>91</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>116</v>
@@ -3720,7 +3843,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>24</v>
       </c>
@@ -3731,13 +3854,14 @@
         <v>2713</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>244</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>25</v>
       </c>
@@ -3748,14 +3872,14 @@
         <v>7375</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1">
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>26</v>
       </c>
@@ -3769,26 +3893,26 @@
         <v>90</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A34" s="38">
+    <row r="34" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="33">
         <v>27</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-    </row>
-    <row r="35" spans="1:9" ht="30.75" thickTop="1">
+      <c r="B34" s="35"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+    </row>
+    <row r="35" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>28</v>
       </c>
@@ -3799,10 +3923,10 @@
         <v>12042</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>108</v>
@@ -3811,7 +3935,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>29</v>
       </c>
@@ -3831,7 +3955,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>30</v>
       </c>
@@ -3842,16 +3966,16 @@
         <v>4932</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>31</v>
       </c>
@@ -3865,13 +3989,13 @@
         <v>77</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>32</v>
       </c>
@@ -3885,7 +4009,7 @@
         <v>77</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>121</v>
@@ -3894,7 +4018,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>33</v>
       </c>
@@ -3908,7 +4032,7 @@
         <v>89</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>117</v>
@@ -3917,7 +4041,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30">
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>34</v>
       </c>
@@ -3931,7 +4055,7 @@
         <v>92</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>109</v>
@@ -3940,27 +4064,27 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>35</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C42" s="8">
         <v>0</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>36</v>
       </c>
@@ -3974,13 +4098,13 @@
         <v>89</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>37</v>
       </c>
@@ -3991,16 +4115,16 @@
         <v>1617</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>38</v>
       </c>
@@ -4011,26 +4135,27 @@
         <v>1488</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A46" s="38">
+        <v>244</v>
+      </c>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="33">
         <v>39</v>
       </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-    </row>
-    <row r="47" spans="1:9" ht="30.75" thickTop="1">
+      <c r="B46" s="35"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+    </row>
+    <row r="47" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>40</v>
       </c>
@@ -4041,10 +4166,10 @@
         <v>15359</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F47" s="15" t="s">
         <v>115</v>
@@ -4056,7 +4181,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="75">
+    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>41</v>
       </c>
@@ -4066,17 +4191,17 @@
       <c r="C48" s="8">
         <v>656</v>
       </c>
-      <c r="D48" s="54" t="s">
-        <v>175</v>
+      <c r="D48" s="49" t="s">
+        <v>171</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F48" s="52" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="45">
+        <v>242</v>
+      </c>
+      <c r="F48" s="47" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>42</v>
       </c>
@@ -4090,16 +4215,16 @@
         <v>84</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>43</v>
       </c>
@@ -4110,27 +4235,27 @@
         <v>989</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>176</v>
+        <v>155</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A51" s="38">
+    <row r="51" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="33">
         <v>44</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
-    </row>
-    <row r="52" spans="1:9" ht="331.5" thickTop="1" thickBot="1">
+      <c r="B51" s="35"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+    </row>
+    <row r="52" spans="1:9" ht="331.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>45</v>
       </c>
@@ -4140,34 +4265,34 @@
       <c r="C52" s="8">
         <v>7069</v>
       </c>
-      <c r="D52" s="51" t="s">
-        <v>240</v>
+      <c r="D52" s="46" t="s">
+        <v>232</v>
       </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="53" t="s">
-        <v>242</v>
+      <c r="F52" s="48" t="s">
+        <v>234</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H52" s="55" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A53" s="38">
+        <v>235</v>
+      </c>
+      <c r="H52" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="33">
         <v>44</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-    </row>
-    <row r="54" spans="1:9" ht="45.75" thickTop="1">
+      <c r="B53" s="35"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+    </row>
+    <row r="54" spans="1:9" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>47</v>
       </c>
@@ -4181,10 +4306,10 @@
         <v>129</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>93</v>
@@ -4193,7 +4318,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>48</v>
       </c>
@@ -4207,13 +4332,13 @@
         <v>84</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>49</v>
       </c>
@@ -4227,10 +4352,13 @@
         <v>76</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="30">
+        <v>246</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>50</v>
       </c>
@@ -4244,13 +4372,13 @@
         <v>66</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>51</v>
       </c>
@@ -4264,33 +4392,33 @@
         <v>66</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F58" s="2"/>
       <c r="H58" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="28">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="23">
         <v>52</v>
       </c>
-      <c r="B59" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E59" s="28"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="B59" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E59" s="23"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>53</v>
       </c>
@@ -4307,7 +4435,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>54</v>
       </c>
@@ -4325,7 +4453,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>55</v>
       </c>
@@ -4343,26 +4471,26 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="28">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="23">
         <v>56</v>
       </c>
-      <c r="B63" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C63" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E63" s="28"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="B63" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E63" s="23"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>57</v>
       </c>
@@ -4373,13 +4501,13 @@
         <v>7134</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>58</v>
       </c>
@@ -4390,16 +4518,16 @@
         <v>99</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>59</v>
       </c>
@@ -4413,10 +4541,10 @@
         <v>68</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="30">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>60</v>
       </c>
@@ -4427,19 +4555,19 @@
         <v>211</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F67" s="27" t="s">
-        <v>197</v>
+        <v>179</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>191</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>66</v>
       </c>
@@ -4450,13 +4578,13 @@
         <v>3054</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>67</v>
       </c>
@@ -4467,16 +4595,16 @@
         <v>4122</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>68</v>
       </c>
@@ -4490,10 +4618,10 @@
         <v>68</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>69</v>
       </c>
@@ -4504,35 +4632,35 @@
         <v>491</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="28">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="23">
         <v>70</v>
       </c>
-      <c r="B72" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C72" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="D72" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E72" s="28"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="28"/>
-      <c r="I72" s="28"/>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="B72" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E72" s="23"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>71</v>
       </c>
@@ -4543,33 +4671,33 @@
         <v>18512</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="E73" s="2"/>
       <c r="G73" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="28">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="23">
         <v>72</v>
       </c>
-      <c r="B74" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C74" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="D74" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E74" s="28"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="B74" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D74" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E74" s="23"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>73</v>
       </c>
@@ -4580,38 +4708,38 @@
         <v>5006</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="28">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="23">
         <v>74</v>
       </c>
-      <c r="B76" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C76" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="D76" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E76" s="28"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="B76" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E76" s="23"/>
+      <c r="F76" s="26"/>
+      <c r="G76" s="26"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>75</v>
       </c>
@@ -4621,32 +4749,34 @@
       <c r="C77" s="8">
         <v>7505</v>
       </c>
-      <c r="D77" s="23"/>
+      <c r="D77" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="E77" s="2"/>
-      <c r="G77" s="24" t="s">
+      <c r="G77" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="28">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="23">
         <v>76</v>
       </c>
-      <c r="B78" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C78" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="D78" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E78" s="28"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="28"/>
-      <c r="I78" s="28"/>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="B78" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C78" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E78" s="23"/>
+      <c r="F78" s="26"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>77</v>
       </c>
@@ -4656,13 +4786,15 @@
       <c r="C79" s="8">
         <v>7403</v>
       </c>
-      <c r="D79" s="22"/>
+      <c r="D79" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="E79" s="2"/>
-      <c r="G79" s="25" t="s">
+      <c r="G79" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>78</v>
       </c>
@@ -4672,13 +4804,15 @@
       <c r="C80" s="8">
         <v>1199</v>
       </c>
-      <c r="D80" s="22"/>
+      <c r="D80" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="E80" s="2"/>
-      <c r="G80" s="25" t="s">
+      <c r="G80" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>79</v>
       </c>
@@ -4688,13 +4822,15 @@
       <c r="C81" s="8">
         <v>5557</v>
       </c>
-      <c r="D81" s="22"/>
+      <c r="D81" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="E81" s="2"/>
-      <c r="G81" s="25" t="s">
+      <c r="G81" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>80</v>
       </c>
@@ -4704,13 +4840,15 @@
       <c r="C82" s="8">
         <v>17898</v>
       </c>
-      <c r="D82" s="22"/>
+      <c r="D82" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="E82" s="2"/>
-      <c r="G82" s="25" t="s">
+      <c r="G82" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>81</v>
       </c>
@@ -4720,344 +4858,355 @@
       <c r="C83" s="8">
         <v>62978</v>
       </c>
-      <c r="D83" s="22"/>
+      <c r="D83" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="E83" s="2"/>
-      <c r="G83" s="26" t="s">
+      <c r="G83" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="28">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="23">
         <v>82</v>
       </c>
-      <c r="B84" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C84" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="D84" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E84" s="28"/>
-      <c r="F84" s="31"/>
-      <c r="G84" s="31"/>
-      <c r="H84" s="28"/>
-      <c r="I84" s="28"/>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="B84" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C84" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D84" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E84" s="23"/>
+      <c r="F84" s="26"/>
+      <c r="G84" s="26"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="23"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D86" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D88" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D89" s="4" t="s">
         <v>126</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D90" s="4" t="s">
         <v>127</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D91" s="4" t="s">
         <v>128</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D92" s="4" t="s">
         <v>131</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D93" s="4" t="s">
         <v>132</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D94" s="4" t="s">
         <v>133</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D95" s="4" t="s">
         <v>134</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D96" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="4:6">
+    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
         <v>136</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="F97" s="2"/>
     </row>
-    <row r="99" spans="4:6">
+    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D99" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E99" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="100" spans="4:6">
+      <c r="E99" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D100" s="4" t="s">
         <v>138</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="101" spans="4:6">
+        <v>247</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D101" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="102" spans="4:6">
+        <v>248</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D102" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="103" spans="4:6">
+        <v>248</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D103" s="4" t="s">
         <v>140</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="105" spans="4:6">
+        <v>248</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D105" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E105" s="18" t="s">
-        <v>141</v>
+      <c r="E105" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="F105" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="4:6">
+    <row r="106" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E106" s="18"/>
     </row>
-    <row r="107" spans="4:6">
+    <row r="107" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D107" s="11" t="s">
         <v>142</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>151</v>
+        <v>238</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="108" spans="4:6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D108" s="11" t="s">
         <v>143</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="109" spans="4:6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D109" s="11" t="s">
         <v>144</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="110" spans="4:6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D110" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="E110" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="F110" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="111" spans="4:6">
+      <c r="E110" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F110" s="51" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D111" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E111" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="F111" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="112" spans="4:6">
+      <c r="E111" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F111" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D112" s="11" t="s">
         <v>147</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="113" spans="4:6">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D113" s="11" t="s">
         <v>148</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="114" spans="4:6">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D114" s="11"/>
       <c r="E114" s="3"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="4:6">
+    <row r="115" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D115" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>166</v>
+        <v>239</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="116" spans="4:6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D116" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>166</v>
+        <v>239</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="117" spans="4:6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D117" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>166</v>
+        <v>239</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="118" spans="4:6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="118" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D118" s="3"/>
       <c r="E118" s="18"/>
     </row>
-    <row r="119" spans="4:6">
+    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D119" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="120" spans="4:6">
+        <v>152</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F119" s="2"/>
+    </row>
+    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D120" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F120" s="2"/>
+    </row>
+    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D121" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E120" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="121" spans="4:6">
-      <c r="D121" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="122" spans="4:6">
+      <c r="E121" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F121" s="2"/>
+    </row>
+    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D122" s="6"/>
       <c r="F122" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D122"/>
+  <autoFilter ref="E1:E122"/>
   <sortState ref="A2:J122">
     <sortCondition ref="A1:A125"/>
   </sortState>
@@ -5077,174 +5226,174 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="147.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="32" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="32" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="32" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="32" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="32" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="32" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="32" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="32" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="32" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="32" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="32" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="32" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="32" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="32" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="32" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="32" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="32" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="32" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="32" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="32" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="32" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="32" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="32" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="32" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="32" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="32" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="32" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="32" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="32" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -5258,7 +5407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
conversion notes for several new functors (F/C/DPHR, CM, RHEM)
</commit_message>
<xml_diff>
--- a/tecto2umr/pdt-c-functors-to-args.xlsx
+++ b/tecto2umr/pdt-c-functors-to-args.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="19050" windowHeight="6705"/>
   </bookViews>
@@ -12,14 +17,14 @@
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$E$1:$E$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$G$1:$G$122</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="265">
   <si>
     <t>RSTR</t>
   </si>
@@ -1404,9 +1409,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>NOT in UMR, NEW to cover this nuance</t>
-  </si>
-  <si>
     <t>NORM</t>
   </si>
   <si>
@@ -1626,14 +1628,6 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT in UMR, NEW to cover EFF
-TODO - nesedí pro slovesa komunikace! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT in UMR, NEW to cover this nuance 
-</t>
   </si>
   <si>
     <t>t_lemma = #Dash, versus, kontra, vs., - , #Separ, tenhle, v, x</t>
@@ -2397,21 +2391,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>TODO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - new abstract concept</t>
-    </r>
-  </si>
-  <si>
     <t>… attribute of quantity/quantity concepts (not relation)</t>
   </si>
   <si>
@@ -2569,13 +2548,366 @@
   <si>
     <t>ARG1 for main clause, ARG2 for contrastive clause
 (?? I would suppose have-contrast-91, rather than contrast-91)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW role, NOT in UMR, NEW to cover EFF
+TODO - nesedí pro slovesa komunikace! </t>
+  </si>
+  <si>
+    <t>NEW role, NOT in UMR, NEW to cover this nuance</t>
+  </si>
+  <si>
+    <t>NEW abstract concept, NOT in UMR, NEW to cover foreign phrases</t>
+  </si>
+  <si>
+    <t>op1, op2, …
+BUT see column F</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In theory, the verb and the CPHR node should be merged … </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>but problem with frame matching</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (many types of coreference between the verb functors and the noub functors)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">!!!
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--&gt; keep it as it is for NOW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TODO - problem with different types of coreference 
+NEEDED inspection of coreference patterns 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(available in VALLEX, not in PDT-Vallex)  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>DPHR-&gt; part-of-phraseme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPHR -&gt; predicative noun </t>
+  </si>
+  <si>
+    <t>concept, abstract entity; plus name role, ops</t>
+  </si>
+  <si>
+    <t>role, NEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO … ?? chceme "zploštit" ?? </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NEW abstract concept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, hyper-role for existing interval entities</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">??? přidat uzel pod #Forn jako společného rodiče  
+a sadu op pro jednotlivé uzly s FPHR 
+                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(to mimic other structures with abstract concepts)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. t_lemma #Forn --&gt; foreign-phrase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (as NEW abstract concept)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. insert </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NEW child</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with relation</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FPHR --&gt; op1, op2, ….</t>
+    </r>
+  </si>
+  <si>
+    <t>CM -&gt; discourse-marker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #Neg -&gt;  attribute "polarity"
+jiné -&gt; tfa marker</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">lemma </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#Neg 194x … jeho rodičem je vždy koord. uzel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (GRAD, ADVS n. CONJ) … </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?? schova</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+??? další t_lemmata … spousty, teď neřešit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(schovat???)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lemma #Neg 27795x  -&gt;  attribute "polarity"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+??? další t_lemmata  … spousty, teď neřešit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(schovat???)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2788,7 +3120,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2939,11 +3271,17 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
-    <cellStyle name="Kontrolní buňka" xfId="2" builtinId="23"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2959,9 +3297,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2999,9 +3337,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3036,7 +3374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3071,7 +3409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3247,25 +3585,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="4"/>
     <col min="3" max="3" width="10" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="62" style="15" customWidth="1"/>
+    <col min="6" max="6" width="57.7109375" style="15" customWidth="1"/>
     <col min="7" max="7" width="67.42578125" style="13" customWidth="1"/>
     <col min="8" max="8" width="44.140625" style="14" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" style="14" customWidth="1"/>
     <col min="10" max="10" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="28">
         <v>0</v>
       </c>
@@ -3297,7 +3635,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3308,10 +3646,10 @@
         <v>10207</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -3322,10 +3660,10 @@
         <v>8427</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -3336,10 +3674,10 @@
         <v>2793</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="6">
         <v>0</v>
       </c>
@@ -3350,11 +3688,11 @@
         <v>209767</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="6">
         <v>0</v>
       </c>
@@ -3365,10 +3703,10 @@
         <v>422</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A7" s="28">
         <v>0</v>
       </c>
@@ -3381,7 +3719,7 @@
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
     </row>
-    <row r="8" spans="1:10" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="120.75" thickTop="1">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -3395,7 +3733,7 @@
         <v>72</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>163</v>
@@ -3404,7 +3742,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="165">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -3418,7 +3756,7 @@
         <v>73</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>164</v>
@@ -3427,7 +3765,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="6">
         <v>3</v>
       </c>
@@ -3441,7 +3779,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>122</v>
@@ -3450,7 +3788,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="60">
       <c r="A11" s="6">
         <v>4</v>
       </c>
@@ -3464,7 +3802,7 @@
         <v>84</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>112</v>
@@ -3479,7 +3817,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30.75" thickBot="1">
       <c r="A12" s="6">
         <v>5</v>
       </c>
@@ -3493,10 +3831,10 @@
         <v>98</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>80</v>
@@ -3505,7 +3843,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A13" s="28">
         <v>6</v>
       </c>
@@ -3518,7 +3856,7 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" thickTop="1">
       <c r="A14" s="6">
         <v>7</v>
       </c>
@@ -3538,7 +3876,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="6">
         <v>8</v>
       </c>
@@ -3552,11 +3890,11 @@
         <v>83</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="6">
         <v>9</v>
       </c>
@@ -3570,13 +3908,13 @@
         <v>82</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="6">
         <v>10</v>
       </c>
@@ -3590,14 +3928,14 @@
         <v>83</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F17" s="2"/>
       <c r="H17" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="6">
         <v>11</v>
       </c>
@@ -3611,11 +3949,11 @@
         <v>103</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="6">
         <v>12</v>
       </c>
@@ -3629,7 +3967,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="6">
         <v>13</v>
       </c>
@@ -3643,7 +3981,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="6">
         <v>14</v>
       </c>
@@ -3657,7 +3995,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1">
       <c r="A22" s="6">
         <v>15</v>
       </c>
@@ -3671,7 +4009,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A23" s="33">
         <v>16</v>
       </c>
@@ -3684,7 +4022,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="1:9" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="75.75" thickTop="1">
       <c r="A24" s="34">
         <v>17</v>
       </c>
@@ -3698,13 +4036,13 @@
         <v>104</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H24" s="44" t="s">
         <v>84</v>
@@ -3713,7 +4051,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="6">
         <v>18</v>
       </c>
@@ -3727,7 +4065,7 @@
         <v>105</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>110</v>
@@ -3739,7 +4077,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="60">
       <c r="A26" s="6">
         <v>19</v>
       </c>
@@ -3753,7 +4091,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>111</v>
@@ -3765,7 +4103,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1">
       <c r="A27" s="6">
         <v>20</v>
       </c>
@@ -3779,7 +4117,7 @@
         <v>67</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>113</v>
@@ -3791,7 +4129,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A28" s="33">
         <v>21</v>
       </c>
@@ -3804,7 +4142,7 @@
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.75" thickTop="1">
       <c r="A29" s="34">
         <v>22</v>
       </c>
@@ -3821,7 +4159,7 @@
       </c>
       <c r="I29" s="44"/>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30">
       <c r="A30" s="6">
         <v>23</v>
       </c>
@@ -3835,7 +4173,7 @@
         <v>91</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>116</v>
@@ -3844,7 +4182,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="6">
         <v>24</v>
       </c>
@@ -3858,11 +4196,11 @@
         <v>156</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="6">
         <v>25</v>
       </c>
@@ -3876,11 +4214,11 @@
         <v>153</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15.75" thickBot="1">
       <c r="A33" s="6">
         <v>26</v>
       </c>
@@ -3894,13 +4232,13 @@
         <v>90</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A34" s="33">
         <v>27</v>
       </c>
@@ -3913,7 +4251,7 @@
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
     </row>
-    <row r="35" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30.75" thickTop="1">
       <c r="A35" s="6">
         <v>28</v>
       </c>
@@ -3924,10 +4262,10 @@
         <v>12042</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>108</v>
@@ -3936,7 +4274,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="6">
         <v>29</v>
       </c>
@@ -3956,7 +4294,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="6">
         <v>30</v>
       </c>
@@ -3970,13 +4308,13 @@
         <v>166</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="6">
         <v>31</v>
       </c>
@@ -3990,13 +4328,13 @@
         <v>77</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="6">
         <v>32</v>
       </c>
@@ -4010,7 +4348,7 @@
         <v>77</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>121</v>
@@ -4019,7 +4357,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="6">
         <v>33</v>
       </c>
@@ -4033,7 +4371,7 @@
         <v>89</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>117</v>
@@ -4042,7 +4380,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="30">
       <c r="A41" s="6">
         <v>34</v>
       </c>
@@ -4056,7 +4394,7 @@
         <v>92</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>109</v>
@@ -4065,12 +4403,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="6">
         <v>35</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C42" s="8">
         <v>0</v>
@@ -4079,13 +4417,13 @@
         <v>166</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="6">
         <v>36</v>
       </c>
@@ -4099,13 +4437,13 @@
         <v>89</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="6">
         <v>37</v>
       </c>
@@ -4116,16 +4454,16 @@
         <v>1617</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1">
       <c r="A45" s="6">
         <v>38</v>
       </c>
@@ -4139,11 +4477,11 @@
         <v>158</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A46" s="33">
         <v>39</v>
       </c>
@@ -4156,7 +4494,7 @@
       <c r="H46" s="33"/>
       <c r="I46" s="33"/>
     </row>
-    <row r="47" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30.75" thickTop="1">
       <c r="A47" s="6">
         <v>40</v>
       </c>
@@ -4167,10 +4505,10 @@
         <v>15359</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F47" s="15" t="s">
         <v>115</v>
@@ -4182,7 +4520,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="75">
       <c r="A48" s="6">
         <v>41</v>
       </c>
@@ -4193,16 +4531,16 @@
         <v>656</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F48" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="45">
       <c r="A49" s="6">
         <v>42</v>
       </c>
@@ -4216,16 +4554,16 @@
         <v>84</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1">
       <c r="A50" s="6">
         <v>43</v>
       </c>
@@ -4239,11 +4577,11 @@
         <v>155</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A51" s="33">
         <v>44</v>
       </c>
@@ -4256,7 +4594,7 @@
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
     </row>
-    <row r="52" spans="1:9" ht="331.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="331.5" thickTop="1" thickBot="1">
       <c r="A52" s="6">
         <v>45</v>
       </c>
@@ -4267,20 +4605,20 @@
         <v>7069</v>
       </c>
       <c r="D52" s="46" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="48" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H52" s="50" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A53" s="33">
         <v>44</v>
       </c>
@@ -4293,7 +4631,7 @@
       <c r="H53" s="33"/>
       <c r="I53" s="33"/>
     </row>
-    <row r="54" spans="1:9" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="45.75" thickTop="1">
       <c r="A54" s="6">
         <v>47</v>
       </c>
@@ -4307,10 +4645,10 @@
         <v>129</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H54" s="14" t="s">
         <v>93</v>
@@ -4319,7 +4657,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="6">
         <v>48</v>
       </c>
@@ -4333,13 +4671,13 @@
         <v>84</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="6">
         <v>49</v>
       </c>
@@ -4353,13 +4691,13 @@
         <v>76</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="30">
       <c r="A57" s="6">
         <v>50</v>
       </c>
@@ -4373,13 +4711,13 @@
         <v>66</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="6">
         <v>51</v>
       </c>
@@ -4393,25 +4731,25 @@
         <v>66</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F58" s="2"/>
       <c r="H58" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="23">
         <v>52</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E59" s="23"/>
       <c r="F59" s="26"/>
@@ -4419,7 +4757,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="75">
       <c r="A60" s="6">
         <v>53</v>
       </c>
@@ -4429,14 +4767,20 @@
       <c r="C60" s="8">
         <v>8959</v>
       </c>
-      <c r="D60" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G60" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D60" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="6">
         <v>54</v>
       </c>
@@ -4446,15 +4790,17 @@
       <c r="C61" s="8">
         <v>5141</v>
       </c>
-      <c r="D61" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="G61" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D61" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="90">
       <c r="A62" s="6">
         <v>55</v>
       </c>
@@ -4464,26 +4810,31 @@
       <c r="C62" s="8">
         <v>59068</v>
       </c>
-      <c r="D62" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="G62" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D62" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F62" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="23">
         <v>56</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E63" s="23"/>
       <c r="F63" s="26"/>
@@ -4491,7 +4842,7 @@
       <c r="H63" s="23"/>
       <c r="I63" s="23"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="6">
         <v>57</v>
       </c>
@@ -4502,13 +4853,13 @@
         <v>7134</v>
       </c>
       <c r="D64" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="6">
         <v>58</v>
       </c>
@@ -4519,16 +4870,16 @@
         <v>99</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="6">
         <v>59</v>
       </c>
@@ -4542,10 +4893,10 @@
         <v>68</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="6">
         <v>60</v>
       </c>
@@ -4556,19 +4907,19 @@
         <v>211</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F67" s="22" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="6">
         <v>66</v>
       </c>
@@ -4579,13 +4930,13 @@
         <v>3054</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="6">
         <v>67</v>
       </c>
@@ -4596,16 +4947,16 @@
         <v>4122</v>
       </c>
       <c r="D69" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G69" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G69" s="17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="6">
         <v>68</v>
       </c>
@@ -4619,10 +4970,10 @@
         <v>68</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="6">
         <v>69</v>
       </c>
@@ -4633,27 +4984,27 @@
         <v>491</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="23">
         <v>70</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E72" s="23"/>
       <c r="F72" s="26"/>
@@ -4661,7 +5012,7 @@
       <c r="H72" s="23"/>
       <c r="I72" s="23"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9">
       <c r="A73" s="6">
         <v>71</v>
       </c>
@@ -4679,18 +5030,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9">
       <c r="A74" s="23">
         <v>72</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C74" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E74" s="23"/>
       <c r="F74" s="26"/>
@@ -4698,7 +5049,7 @@
       <c r="H74" s="23"/>
       <c r="I74" s="23"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9">
       <c r="A75" s="6">
         <v>73</v>
       </c>
@@ -4709,30 +5060,30 @@
         <v>5006</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G75" s="17" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="G75" s="52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="23">
         <v>74</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C76" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E76" s="23"/>
       <c r="F76" s="26"/>
@@ -4740,7 +5091,7 @@
       <c r="H76" s="23"/>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="45">
       <c r="A77" s="6">
         <v>75</v>
       </c>
@@ -4750,26 +5101,31 @@
       <c r="C77" s="8">
         <v>7505</v>
       </c>
-      <c r="D77" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E77" s="2"/>
-      <c r="G77" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D77" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F77" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" s="23">
         <v>76</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E78" s="23"/>
       <c r="F78" s="26"/>
@@ -4777,7 +5133,7 @@
       <c r="H78" s="23"/>
       <c r="I78" s="23"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="A79" s="6">
         <v>77</v>
       </c>
@@ -4795,7 +5151,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" s="6">
         <v>78</v>
       </c>
@@ -4813,7 +5169,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9">
       <c r="A81" s="6">
         <v>79</v>
       </c>
@@ -4831,7 +5187,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9">
       <c r="A82" s="6">
         <v>80</v>
       </c>
@@ -4849,7 +5205,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30">
       <c r="A83" s="6">
         <v>81</v>
       </c>
@@ -4859,26 +5215,29 @@
       <c r="C83" s="8">
         <v>62978</v>
       </c>
-      <c r="D83" s="19" t="s">
-        <v>74</v>
+      <c r="D83" s="17" t="s">
+        <v>262</v>
       </c>
       <c r="E83" s="2"/>
+      <c r="F83" s="53" t="s">
+        <v>264</v>
+      </c>
       <c r="G83" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9">
       <c r="A84" s="23">
         <v>82</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C84" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D84" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E84" s="23"/>
       <c r="F84" s="26"/>
@@ -4886,328 +5245,328 @@
       <c r="H84" s="23"/>
       <c r="I84" s="23"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9">
       <c r="D86" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="D88" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9">
       <c r="D89" s="4" t="s">
         <v>126</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9">
       <c r="D90" s="4" t="s">
         <v>127</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9">
       <c r="D91" s="4" t="s">
         <v>128</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9">
       <c r="D92" s="4" t="s">
         <v>131</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9">
       <c r="D93" s="4" t="s">
         <v>132</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9">
       <c r="D94" s="4" t="s">
         <v>133</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9">
       <c r="D95" s="4" t="s">
         <v>134</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9">
       <c r="D96" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:6">
       <c r="D97" s="4" t="s">
         <v>136</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F97" s="2"/>
     </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:6">
       <c r="D99" s="4" t="s">
         <v>137</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6">
       <c r="D100" s="4" t="s">
         <v>138</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6">
       <c r="D101" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="102" spans="4:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6">
       <c r="D102" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="103" spans="4:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6">
       <c r="D103" s="4" t="s">
         <v>140</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="105" spans="4:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6">
       <c r="D105" s="11" t="s">
         <v>81</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F105" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:6">
       <c r="E106" s="18"/>
     </row>
-    <row r="107" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:6">
       <c r="D107" s="11" t="s">
         <v>142</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="108" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:6">
       <c r="D108" s="11" t="s">
         <v>143</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="109" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:6">
       <c r="D109" s="11" t="s">
         <v>144</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="110" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:6">
       <c r="D110" s="12" t="s">
         <v>145</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F110" s="51" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="111" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6" ht="15.75">
       <c r="D111" s="12" t="s">
         <v>146</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F111" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="112" spans="4:6" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6">
       <c r="D112" s="11" t="s">
         <v>147</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:6">
       <c r="D113" s="11" t="s">
         <v>148</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:6">
       <c r="D114" s="11"/>
       <c r="E114" s="3"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:6">
       <c r="D115" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:6">
       <c r="D116" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:6">
       <c r="D117" s="3" t="s">
         <v>161</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="118" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:6">
       <c r="D118" s="3"/>
       <c r="E118" s="18"/>
     </row>
-    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:6">
       <c r="D119" s="6" t="s">
         <v>152</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F119" s="2"/>
     </row>
-    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:6">
       <c r="D120" s="6" t="s">
         <v>154</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F120" s="2"/>
     </row>
-    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:6">
       <c r="D121" s="6" t="s">
         <v>157</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F121" s="2"/>
     </row>
-    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:6">
       <c r="D122" s="6"/>
       <c r="F122" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E122"/>
+  <autoFilter ref="G1:G122"/>
   <sortState ref="A2:J122">
     <sortCondition ref="A1:A125"/>
   </sortState>
@@ -5227,174 +5586,174 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="147.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="27" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="27" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="27" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" s="27" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="27" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" s="27" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" s="27" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="27" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="27" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" s="27" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" s="27" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" s="27" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" s="27" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" s="27" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="27" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="27" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" s="27" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" s="27" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="27" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" s="27" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" s="27" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" s="27" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" s="27" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" s="27" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+    <row r="27" spans="1:1">
+      <c r="A27" s="27" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="28" spans="1:1">
+      <c r="A28" s="27" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" s="27" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" s="27" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" s="27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+    <row r="32" spans="1:1">
+      <c r="A32" s="27" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" s="27" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -5408,7 +5767,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
functors conversion - comments from others (UMR meeting)
</commit_message>
<xml_diff>
--- a/tecto2umr/pdt-c-functors-to-args.xlsx
+++ b/tecto2umr/pdt-c-functors-to-args.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="274">
   <si>
     <t>funktor</t>
   </si>
@@ -1916,10 +1921,6 @@
     <t>mod</t>
   </si>
   <si>
-    <t>TODO - mod OR part
-?? how directed</t>
-  </si>
-  <si>
     <t>RSTR</t>
   </si>
   <si>
@@ -1927,9 +1928,6 @@
   </si>
   <si>
     <t>CPHR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPHR -&gt; predicative noun </t>
   </si>
   <si>
     <t>role, NEW</t>
@@ -2032,9 +2030,6 @@
     <t>concept, abstract entity; plus name role, ops</t>
   </si>
   <si>
-    <t>NEW abstract concept, NOT in UMR, NEW to cover foreign phrases</t>
-  </si>
-  <si>
     <t>ADVS</t>
   </si>
   <si>
@@ -2133,36 +2128,10 @@
     <t>OPER</t>
   </si>
   <si>
-    <t>interval</t>
-  </si>
-  <si>
     <t>concept, abstract entity; ops</t>
   </si>
   <si>
     <t xml:space="preserve">UMR rozlišuje date-interval, value-interval, between, slash </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>NEW abstract concept</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>, hyper-role for existing interval entities</t>
-    </r>
   </si>
   <si>
     <t>CM</t>
@@ -2980,6 +2949,74 @@
       </rPr>
       <t xml:space="preserve">FPHR --&gt; op1, op2, …. </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO - must be refined
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO - ??? according to, ?? 
+</t>
+  </si>
+  <si>
+    <t>TODO - mod OR part or source
+?? how directed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPHR -&gt; predicative-noun </t>
+  </si>
+  <si>
+    <t>NEW abstract concept, NOT in UMR, NEW to cover foreign phrases
+??? POZOR … FPHR nejso vždy jména</t>
+  </si>
+  <si>
+    <t>NEW role, NOT in UMR, NEW to cover this nuance
+??? conflict (pokud existuje něco takového )</t>
+  </si>
+  <si>
+    <t>gradation</t>
+  </si>
+  <si>
+    <t>NEW keyword, NOT in UMR</t>
+  </si>
+  <si>
+    <r>
+      <t>TODO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> … ??? identity … ??? mod (neměla by tam být negace)</t>
+    </r>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <r>
+      <t>NEW abstract concept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>, hyper-role …. should be refine later</t>
+    </r>
+  </si>
+  <si>
+    <t>TODO … ZKONTROLOVAT, že pod tím nic nevisí (a případně smazat???)</t>
+  </si>
+  <si>
+    <t>NEW role, NOT in UMR, NEW to cover this nuance
+TODO … ZKONTROLOVAT, že pod tím nic nevisí (a případně smazat???)</t>
   </si>
 </sst>
 </file>
@@ -3160,7 +3197,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3197,6 +3234,30 @@
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3227,7 +3288,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3363,11 +3424,26 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Check Cell" xfId="2"/>
-    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3442,6 +3518,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3628,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4446,6 +4525,9 @@
       <c r="F41" s="15" t="s">
         <v>101</v>
       </c>
+      <c r="G41" s="24" t="s">
+        <v>261</v>
+      </c>
       <c r="H41" s="5" t="s">
         <v>100</v>
       </c>
@@ -4470,7 +4552,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>36</v>
       </c>
@@ -4488,6 +4570,9 @@
       </c>
       <c r="F43" s="30" t="s">
         <v>98</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4761,7 +4846,7 @@
         <v>40</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -4769,7 +4854,7 @@
         <v>51</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" s="3">
         <v>493996</v>
@@ -4790,13 +4875,13 @@
         <v>52</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E59" s="36"/>
       <c r="F59" s="36"/>
@@ -4809,22 +4894,22 @@
         <v>53</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C60" s="3">
         <v>8959</v>
       </c>
       <c r="D60" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F60" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="G60" s="16" t="s">
         <v>143</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -4832,19 +4917,19 @@
         <v>54</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C61" s="3">
         <v>5141</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -4852,22 +4937,22 @@
         <v>55</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C62" s="3">
         <v>59068</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F62" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="G62" s="48" t="s">
         <v>265</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -4875,13 +4960,13 @@
         <v>56</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C63" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E63" s="36"/>
       <c r="F63" s="36"/>
@@ -4894,16 +4979,16 @@
         <v>57</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C64" s="3">
         <v>7134</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4911,7 +4996,7 @@
         <v>58</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C65" s="3">
         <v>99</v>
@@ -4923,7 +5008,7 @@
         <v>115</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4931,56 +5016,56 @@
         <v>59</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C66" s="3">
         <v>76346</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>60</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C67" s="3">
         <v>211</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F67" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="F67" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>90</v>
+      <c r="G67" s="48" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>164</v>
+      <c r="B68" s="50" t="s">
+        <v>161</v>
       </c>
       <c r="C68" s="3">
         <v>3054</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -4988,19 +5073,19 @@
         <v>67</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C69" s="3">
         <v>4122</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5008,36 +5093,39 @@
         <v>68</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C70" s="3">
         <v>1346</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>159</v>
+      <c r="D70" s="49" t="s">
+        <v>267</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="G70" s="42" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="11" t="s">
-        <v>170</v>
+      <c r="B71" s="50" t="s">
+        <v>167</v>
       </c>
       <c r="C71" s="3">
         <v>491</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>115</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -5045,13 +5133,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D72" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E72" s="36"/>
       <c r="F72" s="36"/>
@@ -5064,7 +5152,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C73" s="3">
         <v>18512</v>
@@ -5073,8 +5161,8 @@
         <v>86</v>
       </c>
       <c r="E73" s="13"/>
-      <c r="G73" s="29" t="s">
-        <v>86</v>
+      <c r="G73" s="51" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -5082,13 +5170,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C74" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E74" s="36"/>
       <c r="F74" s="36"/>
@@ -5101,22 +5189,22 @@
         <v>73</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C75" s="3">
         <v>5006</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>175</v>
+        <v>270</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="G75" s="18" t="s">
-        <v>178</v>
+        <v>173</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -5124,13 +5212,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C76" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D76" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E76" s="36"/>
       <c r="F76" s="36"/>
@@ -5143,22 +5231,22 @@
         <v>75</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C77" s="3">
         <v>7505</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F77" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="G77" s="18" t="s">
-        <v>90</v>
+        <v>176</v>
+      </c>
+      <c r="G77" s="47" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -5166,13 +5254,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C78" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E78" s="36"/>
       <c r="F78" s="36"/>
@@ -5185,7 +5273,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C79" s="3">
         <v>7403</v>
@@ -5195,7 +5283,7 @@
       </c>
       <c r="E79" s="13"/>
       <c r="G79" s="29" t="s">
-        <v>86</v>
+        <v>272</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -5203,7 +5291,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C80" s="3">
         <v>1199</v>
@@ -5213,7 +5301,7 @@
       </c>
       <c r="E80" s="13"/>
       <c r="G80" s="29" t="s">
-        <v>86</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -5221,7 +5309,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C81" s="3">
         <v>5557</v>
@@ -5231,7 +5319,7 @@
       </c>
       <c r="E81" s="13"/>
       <c r="G81" s="29" t="s">
-        <v>86</v>
+        <v>272</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -5239,7 +5327,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C82" s="3">
         <v>17898</v>
@@ -5249,7 +5337,7 @@
       </c>
       <c r="E82" s="13"/>
       <c r="G82" s="29" t="s">
-        <v>86</v>
+        <v>272</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5257,20 +5345,20 @@
         <v>81</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C83" s="3">
         <v>62978</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E83" s="13"/>
       <c r="F83" s="32" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="G83" s="29" t="s">
-        <v>86</v>
+        <v>272</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -5278,13 +5366,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C84" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D84" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E84" s="36"/>
       <c r="F84" s="36"/>
@@ -5294,18 +5382,18 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D86" s="41" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E86" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F86" s="42" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D88" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>40</v>
@@ -5314,7 +5402,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D89" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>40</v>
@@ -5323,7 +5411,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D90" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>40</v>
@@ -5332,7 +5420,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D91" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>40</v>
@@ -5341,7 +5429,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D92" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>40</v>
@@ -5350,7 +5438,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D93" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>40</v>
@@ -5359,7 +5447,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D94" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>40</v>
@@ -5368,7 +5456,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D95" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>40</v>
@@ -5377,7 +5465,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>40</v>
@@ -5386,7 +5474,7 @@
     </row>
     <row r="97" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D97" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>40</v>
@@ -5395,35 +5483,35 @@
     </row>
     <row r="99" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D99" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E99" s="14" t="s">
         <v>134</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D100" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D101" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="4:6" x14ac:dyDescent="0.25">
@@ -5431,21 +5519,21 @@
         <v>95</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D103" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="4:6" x14ac:dyDescent="0.25">
@@ -5453,10 +5541,10 @@
         <v>36</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F105" s="35" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="106" spans="4:6" x14ac:dyDescent="0.25">
@@ -5464,79 +5552,79 @@
     </row>
     <row r="107" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D107" s="12" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="108" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D108" s="12" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="109" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D109" s="12" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="110" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D110" s="43" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F110" s="44" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="4:6" ht="30.75" x14ac:dyDescent="0.25">
       <c r="D111" s="43" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F111" s="35" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D112" s="12" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F112" s="14" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D113" s="12" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="114" spans="4:6" x14ac:dyDescent="0.25">
@@ -5546,35 +5634,35 @@
     </row>
     <row r="115" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D115" s="13" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D116" s="13" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="117" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D117" s="13" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="118" spans="4:6" x14ac:dyDescent="0.25">
@@ -5583,7 +5671,7 @@
     </row>
     <row r="119" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D119" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E119" s="14" t="s">
         <v>77</v>
@@ -5592,7 +5680,7 @@
     </row>
     <row r="120" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D120" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E120" s="14" t="s">
         <v>77</v>
@@ -5601,7 +5689,7 @@
     </row>
     <row r="121" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D121" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E121" s="14" t="s">
         <v>77</v>
@@ -5637,167 +5725,167 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="45" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="45" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="45" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="45" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
several notes on conversion (UMR Monday meeting)
</commit_message>
<xml_diff>
--- a/tecto2umr/pdt-c-functors-to-args.xlsx
+++ b/tecto2umr/pdt-c-functors-to-args.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="289">
   <si>
     <t>funktor</t>
   </si>
@@ -2040,9 +2040,6 @@
     <t>NOT in PDT-C</t>
   </si>
   <si>
-    <t>considering</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -2142,9 +2139,6 @@
   <si>
     <t xml:space="preserve">TODO - must be further refined
 </t>
-  </si>
-  <si>
-    <t>Śárka's suggestion</t>
   </si>
   <si>
     <t>better name to cover also REG</t>
@@ -2853,121 +2847,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">hrana (e-child) rodič-COMPL --&gt; manner / mod
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>podle sempos rodiče:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   sempos:   v, adj.* --&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>manner</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-                                 n.*  --&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>mod</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-                                 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>undef ... DODĚLAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-(compl.rf šipka) COMPL --&gt; mod-of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-     </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NEBO mod, ale pak od substantiva 
-                                                            k doplňku!!)</t>
-    </r>
-  </si>
-  <si>
     <t>NOT in UMR, NEW keyword</t>
   </si>
   <si>
@@ -2995,10 +2874,6 @@
   </si>
   <si>
     <t>vlastn9 jm0no&lt;&lt;</t>
-  </si>
-  <si>
-    <t>NOT in UMR, NEW  abstract concept
-??? TODO ne vše, co je #Forn ID, je vlastní jméno???</t>
   </si>
   <si>
     <r>
@@ -3035,297 +2910,6 @@
   </si>
   <si>
     <r>
-      <t>!! e-rodič uzlu FPHR má vždy t_lemma #Forn !!
-POKUD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> e-rodič uzlu FPHR (=#Forn)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> není ID </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(6 443x)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   1: t_lemma #Forn 
-        --&gt; foreign-phrase</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (NEW abstract concept)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   2: FPHR --&gt; op1, op2, …. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">     (7x má FPHR dítě
-     1x PAR</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-POKUD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> e-rodič uzlu FPHR  (=#Forn</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) je ID </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(13 449x):</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ID </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(uzlu #Forn) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">--&gt; name </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(role) 
-                                        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>??obecněji  mod</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> t_lemma #Forn --&gt; name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (concept) 
-                                         </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>?? foreign-phrase</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">FPHR --&gt; op1, op2, ….
-       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(2x má FPHR dítě - jednou chyba, 
-                                         podruhé číslovka jako součást jména --&gt; též op)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -3437,24 +3021,28 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>if #Forn NE funktor ID:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
+      <t xml:space="preserve">hrana (e-child) rodič-COMPL --&gt; manner / mod
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>podle sempos rodiče:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
-#Forn --&gt; foreign-phrase
-FPHR --&gt; op1, op2, …
 </t>
     </r>
     <r>
@@ -3463,21 +3051,87 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">   sempos:   v, adj.* --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>manner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">
-if #Forn.ID:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ID --&gt; name / mod
-#Forn --&gt; name 
-                    / foreign-phrase
-FPHR --&gt; op1, op2, …</t>
+                          n.*  --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>mod</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>undef ... DODĚLAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+(compl.rf šipka) COMPL --&gt; mod-of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(NEBO mod, ale pak od substantiva 
+                                                       k doplňku!!)</t>
     </r>
   </si>
   <si>
@@ -3487,14 +3141,399 @@
 subrole (NE) / role (participant)
 concept (abstract entity)
           /concept (abstract entity)
-role (name/foreign-phrase, ops)</t>
+??? (name/foreign-phrase, ops)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>if #Forn NE funktor ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+#Forn --&gt; foreign-phrase
+FPHR --&gt; op1, op2, …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+if #Forn.ID:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ID --&gt; name / mod
+#Forn --&gt; name 
+                    / foreign-phrase
+FPHR --&gt; op1, op2, … ATRIBUTY ??</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>!! e-rodič uzlu FPHR má vždy t_lemma #Forn !!
+POKUD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e-rodič uzlu FPHR (=#Forn)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> není ID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(6 443x)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1: t_lemma #Forn 
+        --&gt; foreign-phrase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (NEW abstract concept)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   2: FPHR --&gt; op1, op2, …. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">     (7x má FPHR dítě
+     1x PAR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+POKUD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e-rodič uzlu FPHR  (=#Forn</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) je ID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(13 449x):</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(uzlu #Forn) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">--&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">name </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(role) ... </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+                                        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>??obecněji  mod</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> t_lemma #Forn --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (concept)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+                                         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>?? foreign-phrase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">FPHR --&gt; op1, op2, …. ATRIBUT místo uzlu
+       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2x má FPHR dítě - jednou chyba, 
+                                         podruhé číslovka jako součást jména --&gt; též op)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>NOT in UMR, NEW  abstract concept
+??? TODO ne vše, co je #Forn ID, je vlastní jméno???
+TODO refinement needed !!!</t>
+  </si>
+  <si>
+    <t>regard</t>
+  </si>
+  <si>
+    <t>Šárka: the same as CRIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3745,8 +3784,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3842,18 +3887,6 @@
         <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -3900,7 +3933,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4025,15 +4058,9 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4043,9 +4070,6 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4071,9 +4095,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4131,13 +4152,7 @@
     <xf numFmtId="0" fontId="21" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4410,64 +4425,64 @@
   <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="3.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="3.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="10" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="73.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="59.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="41.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="73.7265625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="53.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.81640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="23.26953125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="59.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="25">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
-        <v>263</v>
-      </c>
-      <c r="C1" s="71" t="s">
+      <c r="B1" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="71" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" s="73" t="s">
+      <c r="G1" s="67" t="s">
         <v>255</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="H1" s="69" t="s">
         <v>254</v>
       </c>
-      <c r="J1" s="74">
+      <c r="I1" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="J1" s="70">
         <v>2014</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="67" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19">
         <v>0</v>
       </c>
@@ -4488,7 +4503,7 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="19">
         <v>0</v>
       </c>
@@ -4509,7 +4524,7 @@
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="19">
         <v>0</v>
       </c>
@@ -4530,7 +4545,7 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="19">
         <v>0</v>
       </c>
@@ -4551,7 +4566,7 @@
       <c r="J5" s="28"/>
       <c r="K5" s="28"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="19">
         <v>0</v>
       </c>
@@ -4572,7 +4587,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
         <v>0</v>
       </c>
@@ -4587,7 +4602,7 @@
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
     </row>
-    <row r="8" spans="1:12" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="94" x14ac:dyDescent="0.35">
       <c r="A8" s="19">
         <v>1</v>
       </c>
@@ -4602,7 +4617,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G8" s="30"/>
       <c r="H8" s="31" t="s">
@@ -4614,7 +4629,7 @@
       </c>
       <c r="K8" s="28"/>
     </row>
-    <row r="9" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A9" s="19">
         <v>2</v>
       </c>
@@ -4629,7 +4644,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G9" s="30"/>
       <c r="H9" s="31" t="s">
@@ -4641,7 +4656,7 @@
       </c>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="19">
         <v>3</v>
       </c>
@@ -4656,7 +4671,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G10" s="30"/>
       <c r="H10" s="31" t="s">
@@ -4668,7 +4683,7 @@
       </c>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="19">
         <v>4</v>
       </c>
@@ -4683,7 +4698,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G11" s="30"/>
       <c r="H11" s="31" t="s">
@@ -4699,7 +4714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="19">
         <v>5</v>
       </c>
@@ -4714,12 +4729,12 @@
         <v>157</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G12" s="30"/>
       <c r="H12" s="23"/>
       <c r="I12" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J12" s="28" t="s">
         <v>28</v>
@@ -4728,7 +4743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
         <v>6</v>
       </c>
@@ -4743,7 +4758,7 @@
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="19">
         <v>7</v>
       </c>
@@ -4758,7 +4773,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G14" s="30"/>
       <c r="H14" s="23"/>
@@ -4770,7 +4785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="19">
         <v>8</v>
       </c>
@@ -4785,7 +4800,7 @@
         <v>34</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="24"/>
@@ -4793,7 +4808,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="19">
         <v>9</v>
       </c>
@@ -4808,7 +4823,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G16" s="30"/>
       <c r="H16" s="31" t="s">
@@ -4818,7 +4833,7 @@
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="19">
         <v>10</v>
       </c>
@@ -4833,7 +4848,7 @@
         <v>34</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="24"/>
@@ -4843,7 +4858,7 @@
       </c>
       <c r="K17" s="28"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="19">
         <v>11</v>
       </c>
@@ -4858,7 +4873,7 @@
         <v>39</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="24"/>
@@ -4866,7 +4881,7 @@
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="19">
         <v>12</v>
       </c>
@@ -4881,7 +4896,7 @@
         <v>30</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G19" s="30"/>
       <c r="H19" s="23"/>
@@ -4889,7 +4904,7 @@
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="19">
         <v>13</v>
       </c>
@@ -4904,7 +4919,7 @@
         <v>30</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G20" s="30"/>
       <c r="H20" s="23"/>
@@ -4912,7 +4927,7 @@
       <c r="J20" s="28"/>
       <c r="K20" s="28"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="19">
         <v>14</v>
       </c>
@@ -4927,7 +4942,7 @@
         <v>30</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G21" s="30"/>
       <c r="H21" s="23"/>
@@ -4935,7 +4950,7 @@
       <c r="J21" s="28"/>
       <c r="K21" s="28"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="19">
         <v>15</v>
       </c>
@@ -4950,7 +4965,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G22" s="30"/>
       <c r="H22" s="23"/>
@@ -4958,7 +4973,7 @@
       <c r="J22" s="28"/>
       <c r="K22" s="28"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="25">
         <v>16</v>
       </c>
@@ -4973,7 +4988,7 @@
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
     </row>
-    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="19">
         <v>17</v>
       </c>
@@ -4988,7 +5003,7 @@
         <v>45</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G24" s="30"/>
       <c r="H24" s="31" t="s">
@@ -5004,7 +5019,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="19">
         <v>18</v>
       </c>
@@ -5019,7 +5034,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="31" t="s">
@@ -5033,7 +5048,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="19">
         <v>19</v>
       </c>
@@ -5048,7 +5063,7 @@
         <v>55</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G26" s="30"/>
       <c r="H26" s="31" t="s">
@@ -5062,7 +5077,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="19">
         <v>20</v>
       </c>
@@ -5077,7 +5092,7 @@
         <v>60</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G27" s="30"/>
       <c r="H27" s="31" t="s">
@@ -5091,7 +5106,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
         <v>21</v>
       </c>
@@ -5106,7 +5121,7 @@
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="19">
         <v>22</v>
       </c>
@@ -5118,7 +5133,9 @@
       <c r="E29" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="24"/>
+      <c r="F29" s="30" t="s">
+        <v>244</v>
+      </c>
       <c r="G29" s="24"/>
       <c r="H29" s="31" t="s">
         <v>65</v>
@@ -5129,7 +5146,7 @@
       </c>
       <c r="K29" s="28"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="19">
         <v>23</v>
       </c>
@@ -5144,7 +5161,7 @@
         <v>67</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G30" s="30"/>
       <c r="H30" s="31" t="s">
@@ -5156,7 +5173,7 @@
       </c>
       <c r="K30" s="28"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="19">
         <v>24</v>
       </c>
@@ -5171,7 +5188,7 @@
         <v>70</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G31" s="30"/>
       <c r="H31" s="24"/>
@@ -5179,7 +5196,7 @@
       <c r="J31" s="28"/>
       <c r="K31" s="28"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="19">
         <v>25</v>
       </c>
@@ -5194,7 +5211,7 @@
         <v>72</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G32" s="30"/>
       <c r="H32" s="24"/>
@@ -5202,7 +5219,7 @@
       <c r="J32" s="28"/>
       <c r="K32" s="28"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="19">
         <v>26</v>
       </c>
@@ -5217,7 +5234,7 @@
         <v>64</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G33" s="30"/>
       <c r="H33" s="31" t="s">
@@ -5227,7 +5244,7 @@
       <c r="J33" s="28"/>
       <c r="K33" s="28"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="25">
         <v>27</v>
       </c>
@@ -5242,7 +5259,7 @@
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="19">
         <v>28</v>
       </c>
@@ -5257,7 +5274,7 @@
         <v>75</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G35" s="30"/>
       <c r="H35" s="31" t="s">
@@ -5269,7 +5286,7 @@
       </c>
       <c r="K35" s="28"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="19">
         <v>29</v>
       </c>
@@ -5296,7 +5313,7 @@
       </c>
       <c r="K36" s="28"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="19">
         <v>30</v>
       </c>
@@ -5307,23 +5324,23 @@
       <c r="D37" s="21">
         <v>4932</v>
       </c>
-      <c r="E37" s="36" t="s">
-        <v>239</v>
+      <c r="E37" s="62" t="s">
+        <v>287</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="G37" s="80" t="s">
-        <v>259</v>
+        <v>242</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>257</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J37" s="28"/>
       <c r="K37" s="28"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="19">
         <v>31</v>
       </c>
@@ -5338,7 +5355,7 @@
         <v>83</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G38" s="30"/>
       <c r="H38" s="31" t="s">
@@ -5348,7 +5365,7 @@
       <c r="J38" s="28"/>
       <c r="K38" s="28"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="19">
         <v>32</v>
       </c>
@@ -5363,7 +5380,7 @@
         <v>83</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G39" s="30"/>
       <c r="H39" s="31" t="s">
@@ -5375,7 +5392,7 @@
       </c>
       <c r="K39" s="28"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="19">
         <v>33</v>
       </c>
@@ -5390,7 +5407,7 @@
         <v>88</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G40" s="30"/>
       <c r="H40" s="38" t="s">
@@ -5402,7 +5419,7 @@
       </c>
       <c r="K40" s="28"/>
     </row>
-    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="19">
         <v>34</v>
       </c>
@@ -5417,7 +5434,7 @@
         <v>91</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G41" s="30"/>
       <c r="H41" s="31" t="s">
@@ -5431,7 +5448,7 @@
       </c>
       <c r="K41" s="28"/>
     </row>
-    <row r="42" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="39">
         <v>35</v>
       </c>
@@ -5443,22 +5460,22 @@
         <v>0</v>
       </c>
       <c r="E42" s="42" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
       <c r="F42" s="39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G42" s="39"/>
       <c r="H42" s="39" t="s">
         <v>238</v>
       </c>
       <c r="I42" s="43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J42" s="39"/>
       <c r="K42" s="39"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="19">
         <v>36</v>
       </c>
@@ -5469,23 +5486,23 @@
       <c r="D43" s="21">
         <v>10752</v>
       </c>
-      <c r="E43" s="44" t="s">
-        <v>239</v>
+      <c r="E43" s="62" t="s">
+        <v>287</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="G43" s="81" t="s">
-        <v>258</v>
+        <v>242</v>
+      </c>
+      <c r="G43" s="30" t="s">
+        <v>288</v>
       </c>
       <c r="H43" s="23"/>
       <c r="I43" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J43" s="28"/>
       <c r="K43" s="28"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="19">
         <v>37</v>
       </c>
@@ -5500,17 +5517,17 @@
         <v>96</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G44" s="19"/>
       <c r="H44" s="23"/>
       <c r="I44" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J44" s="28"/>
       <c r="K44" s="28"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="19">
         <v>38</v>
       </c>
@@ -5525,7 +5542,7 @@
         <v>98</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G45" s="30"/>
       <c r="H45" s="24"/>
@@ -5533,7 +5550,7 @@
       <c r="J45" s="28"/>
       <c r="K45" s="28"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="25">
         <v>39</v>
       </c>
@@ -5548,7 +5565,7 @@
       <c r="J46" s="25"/>
       <c r="K46" s="25"/>
     </row>
-    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="19">
         <v>40</v>
       </c>
@@ -5563,7 +5580,7 @@
         <v>100</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G47" s="30"/>
       <c r="H47" s="31" t="s">
@@ -5577,11 +5594,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="116" x14ac:dyDescent="0.35">
       <c r="A48" s="19">
         <v>41</v>
       </c>
-      <c r="B48" s="45"/>
+      <c r="B48" s="44"/>
       <c r="C48" s="20" t="s">
         <v>104</v>
       </c>
@@ -5591,18 +5608,18 @@
       <c r="E48" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="F48" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="G48" s="48" t="s">
-        <v>271</v>
+      <c r="F48" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="G48" s="46" t="s">
+        <v>269</v>
       </c>
       <c r="H48" s="23"/>
       <c r="I48" s="19"/>
       <c r="J48" s="28"/>
       <c r="K48" s="28"/>
     </row>
-    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="19">
         <v>42</v>
       </c>
@@ -5617,7 +5634,7 @@
         <v>22</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G49" s="30"/>
       <c r="H49" s="31" t="s">
@@ -5629,7 +5646,7 @@
       <c r="J49" s="28"/>
       <c r="K49" s="28"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="19">
         <v>43</v>
       </c>
@@ -5640,11 +5657,11 @@
       <c r="D50" s="21">
         <v>989</v>
       </c>
-      <c r="E50" s="49" t="s">
+      <c r="E50" s="47" t="s">
         <v>108</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G50" s="30"/>
       <c r="H50" s="24"/>
@@ -5652,7 +5669,7 @@
       <c r="J50" s="28"/>
       <c r="K50" s="28"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="25">
         <v>44</v>
       </c>
@@ -5667,36 +5684,36 @@
       <c r="J51" s="25"/>
       <c r="K51" s="25"/>
     </row>
-    <row r="52" spans="1:11" ht="267" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="267" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="19">
         <v>45</v>
       </c>
-      <c r="B52" s="45"/>
+      <c r="B52" s="44"/>
       <c r="C52" s="20" t="s">
         <v>109</v>
       </c>
       <c r="D52" s="21">
         <v>7069</v>
       </c>
-      <c r="E52" s="50" t="s">
-        <v>253</v>
+      <c r="E52" s="46" t="s">
+        <v>252</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="G52" s="76" t="s">
-        <v>272</v>
-      </c>
-      <c r="H52" s="51" t="s">
-        <v>260</v>
+        <v>281</v>
+      </c>
+      <c r="G52" s="72" t="s">
+        <v>282</v>
+      </c>
+      <c r="H52" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="I52" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J52" s="28"/>
       <c r="K52" s="28"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="25">
         <v>44</v>
       </c>
@@ -5711,7 +5728,7 @@
       <c r="J53" s="25"/>
       <c r="K53" s="25"/>
     </row>
-    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="19">
         <v>47</v>
       </c>
@@ -5726,12 +5743,12 @@
         <v>111</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G54" s="19"/>
       <c r="H54" s="23"/>
       <c r="I54" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J54" s="28" t="s">
         <v>112</v>
@@ -5740,7 +5757,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="19">
         <v>48</v>
       </c>
@@ -5755,17 +5772,17 @@
         <v>22</v>
       </c>
       <c r="F55" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G55" s="30"/>
-      <c r="H55" s="52" t="s">
+      <c r="H55" s="49" t="s">
         <v>115</v>
       </c>
       <c r="I55" s="19"/>
       <c r="J55" s="28"/>
       <c r="K55" s="28"/>
     </row>
-    <row r="56" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="174" x14ac:dyDescent="0.35">
       <c r="A56" s="19">
         <v>49</v>
       </c>
@@ -5776,25 +5793,25 @@
       <c r="D56" s="21">
         <v>38823</v>
       </c>
-      <c r="E56" s="53" t="s">
-        <v>265</v>
+      <c r="E56" s="50" t="s">
+        <v>263</v>
       </c>
       <c r="F56" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="G56" s="75" t="s">
-        <v>285</v>
+        <v>264</v>
+      </c>
+      <c r="G56" s="71" t="s">
+        <v>280</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I56" s="32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J56" s="28"/>
       <c r="K56" s="28"/>
     </row>
-    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="19">
         <v>50</v>
       </c>
@@ -5809,7 +5826,7 @@
         <v>118</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G57" s="19"/>
       <c r="H57" s="23"/>
@@ -5819,7 +5836,7 @@
       <c r="J57" s="28"/>
       <c r="K57" s="28"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="19">
         <v>51</v>
       </c>
@@ -5834,7 +5851,7 @@
         <v>118</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="24"/>
@@ -5844,28 +5861,28 @@
       </c>
       <c r="K58" s="28"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="54">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" s="51">
         <v>52</v>
       </c>
-      <c r="B59" s="54"/>
-      <c r="C59" s="55" t="s">
+      <c r="B59" s="51"/>
+      <c r="C59" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D59" s="56" t="s">
+      <c r="D59" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E59" s="55" t="s">
+      <c r="E59" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F59" s="54"/>
-      <c r="G59" s="54"/>
-      <c r="H59" s="54"/>
-      <c r="I59" s="54"/>
-      <c r="J59" s="54"/>
-      <c r="K59" s="54"/>
-    </row>
-    <row r="60" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
+    </row>
+    <row r="60" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A60" s="19">
         <v>53</v>
       </c>
@@ -5876,8 +5893,8 @@
       <c r="D60" s="21">
         <v>8959</v>
       </c>
-      <c r="E60" s="57" t="s">
-        <v>267</v>
+      <c r="E60" s="54" t="s">
+        <v>265</v>
       </c>
       <c r="F60" s="19" t="s">
         <v>122</v>
@@ -5886,13 +5903,13 @@
       <c r="H60" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="I60" s="58" t="s">
-        <v>269</v>
+      <c r="I60" s="55" t="s">
+        <v>267</v>
       </c>
       <c r="J60" s="28"/>
       <c r="K60" s="28"/>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="19">
         <v>54</v>
       </c>
@@ -5903,21 +5920,21 @@
       <c r="D61" s="21">
         <v>5141</v>
       </c>
-      <c r="E61" s="57" t="s">
-        <v>268</v>
+      <c r="E61" s="54" t="s">
+        <v>266</v>
       </c>
       <c r="F61" s="30" t="s">
         <v>122</v>
       </c>
       <c r="G61" s="30"/>
       <c r="H61" s="23"/>
-      <c r="I61" s="58" t="s">
-        <v>270</v>
+      <c r="I61" s="55" t="s">
+        <v>268</v>
       </c>
       <c r="J61" s="28"/>
       <c r="K61" s="28"/>
     </row>
-    <row r="62" spans="1:11" ht="360" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="319" x14ac:dyDescent="0.35">
       <c r="A62" s="19">
         <v>55</v>
       </c>
@@ -5928,48 +5945,48 @@
       <c r="D62" s="21">
         <v>59068</v>
       </c>
-      <c r="E62" s="79" t="s">
-        <v>287</v>
-      </c>
-      <c r="F62" s="47" t="s">
-        <v>288</v>
-      </c>
-      <c r="G62" s="82" t="s">
+      <c r="E62" s="75" t="s">
         <v>284</v>
       </c>
+      <c r="F62" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="G62" s="76" t="s">
+        <v>285</v>
+      </c>
       <c r="H62" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="I62" s="60" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="I62" s="56" t="s">
+        <v>286</v>
       </c>
       <c r="J62" s="28"/>
       <c r="K62" s="28"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="54">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63" s="51">
         <v>56</v>
       </c>
-      <c r="B63" s="54"/>
-      <c r="C63" s="55" t="s">
+      <c r="B63" s="51"/>
+      <c r="C63" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="56" t="s">
+      <c r="D63" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E63" s="55" t="s">
+      <c r="E63" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="54" t="s">
-        <v>281</v>
-      </c>
-      <c r="J63" s="54"/>
-      <c r="K63" s="54"/>
-    </row>
-    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F63" s="51"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="51" t="s">
+        <v>278</v>
+      </c>
+      <c r="J63" s="51"/>
+      <c r="K63" s="51"/>
+    </row>
+    <row r="64" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="19">
         <v>57</v>
       </c>
@@ -5983,18 +6000,18 @@
       <c r="E64" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="F64" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="G64" s="61"/>
+      <c r="F64" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="G64" s="57"/>
       <c r="H64" s="23" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I64" s="19"/>
       <c r="J64" s="28"/>
       <c r="K64" s="28"/>
     </row>
-    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="19">
         <v>58</v>
       </c>
@@ -6008,10 +6025,10 @@
       <c r="E65" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="F65" s="62" t="s">
-        <v>250</v>
-      </c>
-      <c r="G65" s="62"/>
+      <c r="F65" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="G65" s="58"/>
       <c r="H65" s="30" t="s">
         <v>129</v>
       </c>
@@ -6019,7 +6036,7 @@
       <c r="J65" s="28"/>
       <c r="K65" s="28"/>
     </row>
-    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="19">
         <v>59</v>
       </c>
@@ -6033,16 +6050,16 @@
       <c r="E66" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="F66" s="62" t="s">
-        <v>251</v>
-      </c>
-      <c r="G66" s="62"/>
+      <c r="F66" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G66" s="58"/>
       <c r="H66" s="23"/>
       <c r="I66" s="19"/>
       <c r="J66" s="28"/>
       <c r="K66" s="28"/>
     </row>
-    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="19">
         <v>60</v>
       </c>
@@ -6053,28 +6070,28 @@
       <c r="D67" s="21">
         <v>211</v>
       </c>
-      <c r="E67" s="63" t="s">
+      <c r="E67" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="F67" s="62" t="s">
-        <v>251</v>
-      </c>
-      <c r="G67" s="62"/>
+      <c r="F67" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G67" s="58"/>
       <c r="H67" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="I67" s="59" t="s">
-        <v>242</v>
+      <c r="I67" s="56" t="s">
+        <v>241</v>
       </c>
       <c r="J67" s="28"/>
       <c r="K67" s="28"/>
     </row>
-    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="19">
         <v>66</v>
       </c>
       <c r="B68" s="19"/>
-      <c r="C68" s="64" t="s">
+      <c r="C68" s="60" t="s">
         <v>135</v>
       </c>
       <c r="D68" s="21">
@@ -6083,16 +6100,16 @@
       <c r="E68" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="F68" s="62" t="s">
-        <v>251</v>
-      </c>
-      <c r="G68" s="62"/>
+      <c r="F68" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G68" s="58"/>
       <c r="H68" s="23"/>
       <c r="I68" s="19"/>
       <c r="J68" s="28"/>
       <c r="K68" s="28"/>
     </row>
-    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="19">
         <v>67</v>
       </c>
@@ -6106,18 +6123,18 @@
       <c r="E69" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="F69" s="62" t="s">
-        <v>251</v>
-      </c>
-      <c r="G69" s="62"/>
+      <c r="F69" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G69" s="58"/>
       <c r="H69" s="23"/>
-      <c r="I69" s="65" t="s">
+      <c r="I69" s="61" t="s">
         <v>139</v>
       </c>
       <c r="J69" s="28"/>
       <c r="K69" s="28"/>
     </row>
-    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="19">
         <v>68</v>
       </c>
@@ -6128,26 +6145,26 @@
       <c r="D70" s="21">
         <v>1346</v>
       </c>
-      <c r="E70" s="66" t="s">
+      <c r="E70" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="F70" s="62" t="s">
-        <v>251</v>
-      </c>
-      <c r="G70" s="62"/>
+      <c r="F70" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G70" s="58"/>
       <c r="H70" s="23"/>
       <c r="I70" s="37" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J70" s="28"/>
       <c r="K70" s="28"/>
     </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="19">
         <v>69</v>
       </c>
       <c r="B71" s="19"/>
-      <c r="C71" s="64" t="s">
+      <c r="C71" s="60" t="s">
         <v>141</v>
       </c>
       <c r="D71" s="21">
@@ -6156,10 +6173,10 @@
       <c r="E71" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="F71" s="62" t="s">
-        <v>250</v>
-      </c>
-      <c r="G71" s="62"/>
+      <c r="F71" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="G71" s="58"/>
       <c r="H71" s="30" t="s">
         <v>143</v>
       </c>
@@ -6167,28 +6184,28 @@
       <c r="J71" s="28"/>
       <c r="K71" s="28"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="54">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A72" s="51">
         <v>70</v>
       </c>
-      <c r="B72" s="54"/>
-      <c r="C72" s="55" t="s">
+      <c r="B72" s="51"/>
+      <c r="C72" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D72" s="56" t="s">
+      <c r="D72" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E72" s="55" t="s">
+      <c r="E72" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="54"/>
-      <c r="K72" s="54"/>
-    </row>
-    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="51"/>
+      <c r="J72" s="51"/>
+      <c r="K72" s="51"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="19">
         <v>71</v>
       </c>
@@ -6205,34 +6222,34 @@
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
       <c r="H73" s="23"/>
-      <c r="I73" s="67" t="s">
+      <c r="I73" s="63" t="s">
         <v>233</v>
       </c>
       <c r="J73" s="28"/>
       <c r="K73" s="28"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="54">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A74" s="51">
         <v>72</v>
       </c>
-      <c r="B74" s="54"/>
-      <c r="C74" s="55" t="s">
+      <c r="B74" s="51"/>
+      <c r="C74" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D74" s="56" t="s">
+      <c r="D74" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E74" s="55" t="s">
+      <c r="E74" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F74" s="54"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="54"/>
-    </row>
-    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F74" s="51"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="51"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="51"/>
+      <c r="K74" s="51"/>
+    </row>
+    <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="19">
         <v>73</v>
       </c>
@@ -6243,13 +6260,13 @@
       <c r="D75" s="21">
         <v>5006</v>
       </c>
-      <c r="E75" s="63" t="s">
+      <c r="E75" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="F75" s="62" t="s">
-        <v>251</v>
-      </c>
-      <c r="G75" s="62"/>
+      <c r="F75" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G75" s="58"/>
       <c r="H75" s="30" t="s">
         <v>146</v>
       </c>
@@ -6259,28 +6276,28 @@
       <c r="J75" s="28"/>
       <c r="K75" s="28"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="54">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A76" s="51">
         <v>74</v>
       </c>
-      <c r="B76" s="54"/>
-      <c r="C76" s="55" t="s">
+      <c r="B76" s="51"/>
+      <c r="C76" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D76" s="56" t="s">
+      <c r="D76" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E76" s="55" t="s">
+      <c r="E76" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="54"/>
-      <c r="J76" s="54"/>
-      <c r="K76" s="54"/>
-    </row>
-    <row r="77" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F76" s="51"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="51"/>
+      <c r="I76" s="51"/>
+      <c r="J76" s="51"/>
+      <c r="K76" s="51"/>
+    </row>
+    <row r="77" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="19">
         <v>75</v>
       </c>
@@ -6291,44 +6308,44 @@
       <c r="D77" s="21">
         <v>7505</v>
       </c>
-      <c r="E77" s="65" t="s">
+      <c r="E77" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="F77" s="68" t="s">
+      <c r="F77" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="G77" s="68"/>
-      <c r="H77" s="69" t="s">
+      <c r="G77" s="64"/>
+      <c r="H77" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="I77" s="70" t="s">
+      <c r="I77" s="66" t="s">
         <v>237</v>
       </c>
       <c r="J77" s="28"/>
       <c r="K77" s="28"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="54">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A78" s="51">
         <v>76</v>
       </c>
-      <c r="B78" s="54"/>
-      <c r="C78" s="55" t="s">
+      <c r="B78" s="51"/>
+      <c r="C78" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D78" s="56" t="s">
+      <c r="D78" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E78" s="55" t="s">
+      <c r="E78" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F78" s="54"/>
-      <c r="G78" s="54"/>
-      <c r="H78" s="54"/>
-      <c r="I78" s="54"/>
-      <c r="J78" s="54"/>
-      <c r="K78" s="54"/>
-    </row>
-    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F78" s="51"/>
+      <c r="G78" s="51"/>
+      <c r="H78" s="51"/>
+      <c r="I78" s="51"/>
+      <c r="J78" s="51"/>
+      <c r="K78" s="51"/>
+    </row>
+    <row r="79" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="19">
         <v>77</v>
       </c>
@@ -6351,7 +6368,7 @@
       <c r="J79" s="28"/>
       <c r="K79" s="28"/>
     </row>
-    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="19">
         <v>78</v>
       </c>
@@ -6374,7 +6391,7 @@
       <c r="J80" s="28"/>
       <c r="K80" s="28"/>
     </row>
-    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="19">
         <v>79</v>
       </c>
@@ -6397,7 +6414,7 @@
       <c r="J81" s="28"/>
       <c r="K81" s="28"/>
     </row>
-    <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="19">
         <v>80</v>
       </c>
@@ -6420,7 +6437,7 @@
       <c r="J82" s="28"/>
       <c r="K82" s="28"/>
     </row>
-    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="19">
         <v>81</v>
       </c>
@@ -6431,12 +6448,12 @@
       <c r="D83" s="21">
         <v>62978</v>
       </c>
-      <c r="E83" s="65" t="s">
+      <c r="E83" s="61" t="s">
         <v>155</v>
       </c>
       <c r="F83" s="24"/>
       <c r="G83" s="24"/>
-      <c r="H83" s="48" t="s">
+      <c r="H83" s="46" t="s">
         <v>156</v>
       </c>
       <c r="I83" s="35" t="s">
@@ -6445,206 +6462,206 @@
       <c r="J83" s="28"/>
       <c r="K83" s="28"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="54">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A84" s="51">
         <v>82</v>
       </c>
-      <c r="B84" s="54"/>
-      <c r="C84" s="55" t="s">
+      <c r="B84" s="51"/>
+      <c r="C84" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D84" s="56" t="s">
+      <c r="D84" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E84" s="55" t="s">
+      <c r="E84" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F84" s="54"/>
-      <c r="G84" s="54"/>
-      <c r="H84" s="54"/>
-      <c r="I84" s="54"/>
-      <c r="J84" s="54"/>
-      <c r="K84" s="54"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F84" s="51"/>
+      <c r="G84" s="51"/>
+      <c r="H84" s="51"/>
+      <c r="I84" s="51"/>
+      <c r="J84" s="51"/>
+      <c r="K84" s="51"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E86" s="13" t="s">
         <v>157</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G86" s="12"/>
       <c r="H86" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E88" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H88" s="8"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E89" s="2" t="s">
         <v>160</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H89" s="8"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E90" s="2" t="s">
         <v>161</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E91" s="2" t="s">
         <v>162</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H91" s="8"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E92" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H92" s="8"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E93" s="2" t="s">
         <v>164</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H93" s="8"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E94" s="2" t="s">
         <v>165</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H94" s="8"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E95" s="2" t="s">
         <v>166</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H95" s="8"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E96" s="2" t="s">
         <v>167</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H96" s="8"/>
     </row>
-    <row r="97" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E97" s="2" t="s">
         <v>168</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H97" s="8"/>
     </row>
-    <row r="99" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E99" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G99" s="12"/>
       <c r="H99" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="100" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E100" s="2" t="s">
         <v>171</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G100" s="8"/>
       <c r="H100" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="101" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E101" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G101" s="8"/>
       <c r="H101" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="102" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E102" s="2" t="s">
         <v>86</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G102" s="8"/>
       <c r="H102" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="103" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E103" s="2" t="s">
         <v>174</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G103" s="8"/>
       <c r="H103" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="105" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E105" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G105" s="8"/>
       <c r="H105" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:8" x14ac:dyDescent="0.35">
       <c r="F106" s="10"/>
       <c r="G106" s="10"/>
     </row>
-    <row r="107" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E107" s="7" t="s">
         <v>176</v>
       </c>
@@ -6656,7 +6673,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="108" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E108" s="7" t="s">
         <v>179</v>
       </c>
@@ -6668,7 +6685,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="109" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E109" s="7" t="s">
         <v>181</v>
       </c>
@@ -6680,7 +6697,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="110" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E110" s="15" t="s">
         <v>183</v>
       </c>
@@ -6692,7 +6709,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="111" spans="5:8" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:8" ht="30" x14ac:dyDescent="0.35">
       <c r="E111" s="15" t="s">
         <v>185</v>
       </c>
@@ -6704,7 +6721,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="112" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E112" s="7" t="s">
         <v>187</v>
       </c>
@@ -6716,7 +6733,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="113" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E113" s="7" t="s">
         <v>189</v>
       </c>
@@ -6728,13 +6745,13 @@
         <v>188</v>
       </c>
     </row>
-    <row r="114" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E114" s="7"/>
       <c r="F114" s="8"/>
       <c r="G114" s="8"/>
       <c r="H114" s="8"/>
     </row>
-    <row r="115" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E115" s="8" t="s">
         <v>190</v>
       </c>
@@ -6746,7 +6763,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="116" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E116" s="8" t="s">
         <v>192</v>
       </c>
@@ -6758,7 +6775,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="117" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E117" s="8" t="s">
         <v>193</v>
       </c>
@@ -6770,42 +6787,42 @@
         <v>191</v>
       </c>
     </row>
-    <row r="118" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E118" s="8"/>
       <c r="F118" s="10"/>
       <c r="G118" s="10"/>
     </row>
-    <row r="119" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E119" s="1" t="s">
         <v>194</v>
       </c>
       <c r="F119" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G119" s="12"/>
       <c r="H119" s="8"/>
     </row>
-    <row r="120" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E120" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F120" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G120" s="12"/>
       <c r="H120" s="8"/>
     </row>
-    <row r="121" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E121" s="1" t="s">
         <v>196</v>
       </c>
       <c r="F121" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G121" s="12"/>
       <c r="H121" s="8"/>
     </row>
-    <row r="122" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E122" s="1"/>
       <c r="H122" s="8"/>
     </row>
@@ -6827,33 +6844,33 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="58.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="73" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="C2" s="73" t="s">
         <v>276</v>
-      </c>
-      <c r="C1" s="78" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B2" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="C2" s="77" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -6870,172 +6887,172 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="147.140625" customWidth="1"/>
+    <col min="1" max="1" width="147.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
PDT functors (small comment)
</commit_message>
<xml_diff>
--- a/tecto2umr/pdt-c-functors-to-args.xlsx
+++ b/tecto2umr/pdt-c-functors-to-args.xlsx
@@ -4425,8 +4425,8 @@
   <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
more on "mode" attribute
</commit_message>
<xml_diff>
--- a/tecto2umr/pdt-c-functors-to-args.xlsx
+++ b/tecto2umr/pdt-c-functors-to-args.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="835" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="835" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="funktory" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3706" uniqueCount="1848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3710" uniqueCount="1851">
   <si>
     <t>HŠ</t>
   </si>
@@ -13957,9 +13957,6 @@
     <t>nemá UMR protiklad (NE expressive)</t>
   </si>
   <si>
-    <t>nemá UMR protiklad</t>
-  </si>
-  <si>
     <t>:POLARITY -</t>
   </si>
   <si>
@@ -15132,6 +15129,138 @@
   </si>
   <si>
     <t>More subtle analysis in PDT (not used in the conversion):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guidelines: 
+You must go there! = Go there! 
+Could you close the window? = cose the window! </t>
+  </si>
+  <si>
+    <t>t-node $rodic :=
+[sentmod = "enunc", 
+gram/deontmod = "deb",
+gram/tense = "post", 
+gram/factmod != "irreal",
+echild t-node 
+[functor = "ACT", gram/person != "1"]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enunc 
+a na základě gramatémů najít kandidáty
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">??? též gram/deontmod = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"hrt"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>NEE!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+??? též gram/deontmod = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"perm"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+ale navíc s negací pod rodičem
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NEE!!
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">??? též gram/deontmod = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"poss"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+ale navíc s negací pod rodičem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Spíš NE (typ "nedá se s tím počítat")</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -16008,7 +16137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -16325,6 +16454,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -16333,7 +16473,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="389">
+  <cellXfs count="396">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -16911,9 +17051,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -17031,36 +17168,6 @@
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="69" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="3" applyBorder="1"/>
@@ -17199,56 +17306,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="3" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -17318,6 +17380,99 @@
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="74" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -19273,7 +19428,7 @@
         <v>160</v>
       </c>
       <c r="H61" s="22"/>
-      <c r="I61" s="277" t="s">
+      <c r="I61" s="276" t="s">
         <v>1726</v>
       </c>
       <c r="J61" s="24" t="s">
@@ -20686,7 +20841,7 @@
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D1" s="119" t="s">
         <v>734</v>
@@ -21219,7 +21374,7 @@
       <c r="M16" s="121" t="s">
         <v>877</v>
       </c>
-      <c r="N16" s="276" t="s">
+      <c r="N16" s="275" t="s">
         <v>878</v>
       </c>
     </row>
@@ -21257,7 +21412,7 @@
       <c r="M17" s="121" t="s">
         <v>880</v>
       </c>
-      <c r="N17" s="276" t="s">
+      <c r="N17" s="275" t="s">
         <v>881</v>
       </c>
     </row>
@@ -21295,7 +21450,7 @@
       <c r="M18" s="121" t="s">
         <v>883</v>
       </c>
-      <c r="N18" s="276" t="s">
+      <c r="N18" s="275" t="s">
         <v>884</v>
       </c>
     </row>
@@ -21333,7 +21488,7 @@
       <c r="M19" s="121" t="s">
         <v>886</v>
       </c>
-      <c r="N19" s="276" t="s">
+      <c r="N19" s="275" t="s">
         <v>887</v>
       </c>
     </row>
@@ -26449,380 +26604,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="302" t="s">
+      <c r="B1" s="291" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C1" s="291" t="s">
         <v>1744</v>
       </c>
-      <c r="C1" s="302" t="s">
+      <c r="D1" s="291" t="s">
         <v>1745</v>
       </c>
-      <c r="D1" s="302" t="s">
+      <c r="E1" s="291" t="s">
         <v>1746</v>
       </c>
-      <c r="E1" s="302" t="s">
+      <c r="F1" s="180" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="296" t="s">
+        <v>873</v>
+      </c>
+      <c r="B2" s="292" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C2" s="299" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D2" s="299" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E2" s="300" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F2" s="288" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="305" t="s">
         <v>1747</v>
       </c>
-      <c r="F1" s="180" t="s">
+      <c r="B3" s="306" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C3" s="307" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D3" s="307" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E3" s="308" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F3" s="309" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="298" t="s">
+        <v>639</v>
+      </c>
+      <c r="B4" s="292" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C4" s="324" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D4" s="324" t="s">
+        <v>325</v>
+      </c>
+      <c r="E4" s="325" t="s">
+        <v>1771</v>
+      </c>
+      <c r="F4" s="259" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="298" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B5" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C5" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="323" t="s">
+        <v>325</v>
+      </c>
+      <c r="F5" s="259" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="298" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B6" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C6" s="322" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D6" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="E6" s="323" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F6" s="259" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="298" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B7" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C7" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="D7" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="E7" s="323" t="s">
+        <v>325</v>
+      </c>
+      <c r="F7" s="259" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="298" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B8" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C8" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="E8" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="F8" s="259" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="298" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B9" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C9" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="E9" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="F9" s="259" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="298" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B10" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C10" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="D10" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="E10" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="F10" s="290" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="298" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B11" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C11" s="322" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D11" s="322" t="s">
+        <v>325</v>
+      </c>
+      <c r="E11" s="323" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F11" s="259" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="297" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B12" s="293" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C12" s="326" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D12" s="326" t="s">
+        <v>325</v>
+      </c>
+      <c r="E12" s="327" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F12" s="289" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="298" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="292" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C13" s="299" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D13" s="314" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="300" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F13" s="259" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="298" t="s">
+        <v>858</v>
+      </c>
+      <c r="B14" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C14" s="303" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D14" s="312" t="s">
+        <v>325</v>
+      </c>
+      <c r="E14" s="304" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F14" s="259" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="298" t="s">
         <v>1766</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="307" t="s">
-        <v>873</v>
-      </c>
-      <c r="B2" s="303" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C2" s="310" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D2" s="310" t="s">
-        <v>1774</v>
-      </c>
-      <c r="E2" s="311" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F2" s="299" t="s">
+      <c r="B15" s="294" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C15" s="312" t="s">
+        <v>325</v>
+      </c>
+      <c r="D15" s="312" t="s">
+        <v>325</v>
+      </c>
+      <c r="E15" s="311" t="s">
+        <v>325</v>
+      </c>
+      <c r="F15" s="259" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="298" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B16" s="295" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C16" s="312" t="s">
+        <v>325</v>
+      </c>
+      <c r="D16" s="312" t="s">
+        <v>325</v>
+      </c>
+      <c r="E16" s="311" t="s">
+        <v>325</v>
+      </c>
+      <c r="F16" s="259" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="310" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B17" s="316" t="s">
+        <v>325</v>
+      </c>
+      <c r="C17" s="303" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D17" s="312" t="s">
+        <v>325</v>
+      </c>
+      <c r="E17" s="304" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F17" s="315" t="s">
         <v>1776</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="316" t="s">
-        <v>1748</v>
-      </c>
-      <c r="B3" s="317" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C3" s="318" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D3" s="318" t="s">
-        <v>1774</v>
-      </c>
-      <c r="E3" s="319" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F3" s="320" t="s">
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="309" t="s">
-        <v>639</v>
-      </c>
-      <c r="B4" s="303" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C4" s="335" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D4" s="335" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="298" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B18" s="295" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C18" s="303" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D18" s="312" t="s">
         <v>325</v>
       </c>
-      <c r="E4" s="336" t="s">
-        <v>1772</v>
-      </c>
-      <c r="F4" s="260" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="309" t="s">
-        <v>1775</v>
-      </c>
-      <c r="B5" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C5" s="333" t="s">
+      <c r="E18" s="304" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F18" s="259" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="297" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B19" s="293" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C19" s="301" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D19" s="313" t="s">
         <v>325</v>
       </c>
-      <c r="D5" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="E5" s="334" t="s">
-        <v>325</v>
-      </c>
-      <c r="F5" s="260" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="309" t="s">
-        <v>1750</v>
-      </c>
-      <c r="B6" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C6" s="333" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D6" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="E6" s="334" t="s">
+      <c r="E19" s="302" t="s">
         <v>1773</v>
       </c>
-      <c r="F6" s="260" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="309" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B7" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C7" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="D7" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="E7" s="334" t="s">
-        <v>325</v>
-      </c>
-      <c r="F7" s="260" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="309" t="s">
-        <v>1752</v>
-      </c>
-      <c r="B8" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C8" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="D8" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="E8" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="F8" s="260" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="309" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B9" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C9" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="D9" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="E9" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="F9" s="260" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="309" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B10" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C10" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="D10" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="E10" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="F10" s="301" t="s">
-        <v>1762</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="309" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B11" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C11" s="333" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D11" s="333" t="s">
-        <v>325</v>
-      </c>
-      <c r="E11" s="334" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F11" s="260" t="s">
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="308" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B12" s="304" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C12" s="337" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D12" s="337" t="s">
-        <v>325</v>
-      </c>
-      <c r="E12" s="338" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F12" s="300" t="s">
+      <c r="F19" s="289" t="s">
         <v>1764</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="309" t="s">
-        <v>290</v>
-      </c>
-      <c r="B13" s="303" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C13" s="310" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D13" s="325" t="s">
-        <v>325</v>
-      </c>
-      <c r="E13" s="311" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F13" s="260" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="309" t="s">
-        <v>858</v>
-      </c>
-      <c r="B14" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C14" s="314" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D14" s="323" t="s">
-        <v>325</v>
-      </c>
-      <c r="E14" s="315" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F14" s="260" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="309" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B15" s="305" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C15" s="323" t="s">
-        <v>325</v>
-      </c>
-      <c r="D15" s="323" t="s">
-        <v>325</v>
-      </c>
-      <c r="E15" s="322" t="s">
-        <v>325</v>
-      </c>
-      <c r="F15" s="260" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="309" t="s">
-        <v>1770</v>
-      </c>
-      <c r="B16" s="306" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C16" s="323" t="s">
-        <v>325</v>
-      </c>
-      <c r="D16" s="323" t="s">
-        <v>325</v>
-      </c>
-      <c r="E16" s="322" t="s">
-        <v>325</v>
-      </c>
-      <c r="F16" s="260" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="321" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B17" s="327" t="s">
-        <v>325</v>
-      </c>
-      <c r="C17" s="314" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D17" s="323" t="s">
-        <v>325</v>
-      </c>
-      <c r="E17" s="315" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F17" s="326" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="309" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B18" s="306" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C18" s="314" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D18" s="323" t="s">
-        <v>325</v>
-      </c>
-      <c r="E18" s="315" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F18" s="260" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="308" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B19" s="304" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C19" s="312" t="s">
-        <v>1774</v>
-      </c>
-      <c r="D19" s="324" t="s">
-        <v>325</v>
-      </c>
-      <c r="E19" s="313" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F19" s="300" t="s">
-        <v>1765</v>
       </c>
     </row>
   </sheetData>
@@ -26898,10 +27053,10 @@
       <c r="D4" s="131" t="s">
         <v>1168</v>
       </c>
-      <c r="F4" s="278" t="s">
+      <c r="F4" s="368" t="s">
         <v>904</v>
       </c>
-      <c r="G4" s="279"/>
+      <c r="G4" s="369"/>
       <c r="H4" s="132" t="s">
         <v>905</v>
       </c>
@@ -26923,8 +27078,8 @@
       <c r="D5" s="131" t="s">
         <v>1168</v>
       </c>
-      <c r="F5" s="278"/>
-      <c r="G5" s="279"/>
+      <c r="F5" s="368"/>
+      <c r="G5" s="369"/>
       <c r="H5" s="135"/>
       <c r="I5" s="136"/>
       <c r="J5" s="136"/>
@@ -26935,8 +27090,8 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="131"/>
       <c r="D6" s="131"/>
-      <c r="F6" s="278"/>
-      <c r="G6" s="279"/>
+      <c r="F6" s="368"/>
+      <c r="G6" s="369"/>
       <c r="H6" s="138"/>
       <c r="I6" s="139" t="s">
         <v>910</v>
@@ -26959,10 +27114,10 @@
       <c r="E7" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="F7" s="278" t="s">
+      <c r="F7" s="368" t="s">
         <v>912</v>
       </c>
-      <c r="G7" s="278" t="s">
+      <c r="G7" s="368" t="s">
         <v>913</v>
       </c>
       <c r="H7" s="141" t="s">
@@ -26987,8 +27142,8 @@
       <c r="E8" s="170" t="s">
         <v>909</v>
       </c>
-      <c r="F8" s="278"/>
-      <c r="G8" s="278"/>
+      <c r="F8" s="368"/>
+      <c r="G8" s="368"/>
       <c r="H8" s="144"/>
       <c r="I8" s="145"/>
       <c r="J8" s="146" t="s">
@@ -27009,8 +27164,8 @@
         <v>1278</v>
       </c>
       <c r="E9" s="170"/>
-      <c r="F9" s="278"/>
-      <c r="G9" s="278"/>
+      <c r="F9" s="368"/>
+      <c r="G9" s="368"/>
       <c r="H9" s="144"/>
       <c r="I9" s="145"/>
       <c r="J9" s="146"/>
@@ -27031,8 +27186,8 @@
       <c r="E10" s="127" t="s">
         <v>916</v>
       </c>
-      <c r="F10" s="278"/>
-      <c r="G10" s="278"/>
+      <c r="F10" s="368"/>
+      <c r="G10" s="368"/>
       <c r="H10" s="144"/>
       <c r="I10" s="145"/>
       <c r="J10" s="146" t="s">
@@ -27055,8 +27210,8 @@
       <c r="E11" s="170" t="s">
         <v>1501</v>
       </c>
-      <c r="F11" s="278"/>
-      <c r="G11" s="278"/>
+      <c r="F11" s="368"/>
+      <c r="G11" s="368"/>
       <c r="H11" s="144"/>
       <c r="I11" s="145"/>
       <c r="J11" s="146"/>
@@ -27077,8 +27232,8 @@
       <c r="E12" s="170" t="s">
         <v>1501</v>
       </c>
-      <c r="F12" s="278"/>
-      <c r="G12" s="278"/>
+      <c r="F12" s="368"/>
+      <c r="G12" s="368"/>
       <c r="H12" s="151"/>
       <c r="I12" s="152"/>
       <c r="J12" s="153" t="s">
@@ -27101,8 +27256,8 @@
       <c r="E13" s="170" t="s">
         <v>1501</v>
       </c>
-      <c r="F13" s="278"/>
-      <c r="G13" s="280" t="s">
+      <c r="F13" s="368"/>
+      <c r="G13" s="370" t="s">
         <v>927</v>
       </c>
       <c r="H13" s="155" t="s">
@@ -27127,8 +27282,8 @@
       <c r="E14" s="127" t="s">
         <v>923</v>
       </c>
-      <c r="F14" s="278"/>
-      <c r="G14" s="280"/>
+      <c r="F14" s="368"/>
+      <c r="G14" s="370"/>
       <c r="H14" s="157"/>
       <c r="I14" s="157"/>
       <c r="J14" s="157" t="s">
@@ -27149,8 +27304,8 @@
       <c r="E15" s="127" t="s">
         <v>925</v>
       </c>
-      <c r="F15" s="278"/>
-      <c r="G15" s="280"/>
+      <c r="F15" s="368"/>
+      <c r="G15" s="370"/>
       <c r="H15" s="157"/>
       <c r="I15" s="157"/>
       <c r="J15" s="159" t="s">
@@ -27173,8 +27328,8 @@
       <c r="E16" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="F16" s="278"/>
-      <c r="G16" s="280"/>
+      <c r="F16" s="368"/>
+      <c r="G16" s="370"/>
       <c r="H16" s="160"/>
       <c r="I16" s="160"/>
       <c r="J16" s="161" t="s">
@@ -27197,8 +27352,8 @@
       <c r="E17" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="F17" s="278"/>
-      <c r="G17" s="280"/>
+      <c r="F17" s="368"/>
+      <c r="G17" s="370"/>
       <c r="H17" s="157"/>
       <c r="I17" s="157"/>
       <c r="J17" s="157"/>
@@ -27219,8 +27374,8 @@
       <c r="E18" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="F18" s="278"/>
-      <c r="G18" s="280"/>
+      <c r="F18" s="368"/>
+      <c r="G18" s="370"/>
       <c r="H18" s="157"/>
       <c r="I18" s="157"/>
       <c r="J18" s="157"/>
@@ -27239,8 +27394,8 @@
       <c r="E19" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="F19" s="278"/>
-      <c r="G19" s="280"/>
+      <c r="F19" s="368"/>
+      <c r="G19" s="370"/>
       <c r="H19" s="164"/>
       <c r="I19" s="164"/>
       <c r="J19" s="164" t="s">
@@ -27325,7 +27480,7 @@
       <c r="E24" s="127" t="s">
         <v>939</v>
       </c>
-      <c r="H24" s="281" t="s">
+      <c r="H24" s="363" t="s">
         <v>943</v>
       </c>
       <c r="I24" s="149" t="s">
@@ -27346,7 +27501,7 @@
       <c r="E25" s="170" t="s">
         <v>1400</v>
       </c>
-      <c r="H25" s="281"/>
+      <c r="H25" s="363"/>
       <c r="I25" s="167" t="s">
         <v>946</v>
       </c>
@@ -27365,7 +27520,7 @@
       <c r="E26" s="170" t="s">
         <v>909</v>
       </c>
-      <c r="H26" s="281"/>
+      <c r="H26" s="363"/>
       <c r="I26" s="167" t="s">
         <v>947</v>
       </c>
@@ -27384,7 +27539,7 @@
       <c r="E27" s="166" t="s">
         <v>941</v>
       </c>
-      <c r="H27" s="281"/>
+      <c r="H27" s="363"/>
       <c r="I27" s="167" t="s">
         <v>948</v>
       </c>
@@ -27403,7 +27558,7 @@
       <c r="E28" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="H28" s="281"/>
+      <c r="H28" s="363"/>
       <c r="I28" s="167" t="s">
         <v>949</v>
       </c>
@@ -27422,7 +27577,7 @@
       <c r="E29" s="127" t="s">
         <v>945</v>
       </c>
-      <c r="H29" s="281"/>
+      <c r="H29" s="363"/>
       <c r="I29" s="167" t="s">
         <v>951</v>
       </c>
@@ -27441,7 +27596,7 @@
       <c r="E30" s="170" t="s">
         <v>909</v>
       </c>
-      <c r="H30" s="281"/>
+      <c r="H30" s="363"/>
       <c r="I30" s="167" t="s">
         <v>953</v>
       </c>
@@ -27519,8 +27674,8 @@
       <c r="E35" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="H35" s="282"/>
-      <c r="I35" s="283" t="s">
+      <c r="H35" s="364"/>
+      <c r="I35" s="365" t="s">
         <v>956</v>
       </c>
       <c r="J35" s="167" t="s">
@@ -27540,8 +27695,8 @@
       <c r="E36" s="170" t="s">
         <v>909</v>
       </c>
-      <c r="H36" s="282"/>
-      <c r="I36" s="282"/>
+      <c r="H36" s="364"/>
+      <c r="I36" s="364"/>
       <c r="J36" s="167" t="s">
         <v>959</v>
       </c>
@@ -27559,8 +27714,8 @@
       <c r="E37" s="170" t="s">
         <v>909</v>
       </c>
-      <c r="H37" s="282"/>
-      <c r="I37" s="282"/>
+      <c r="H37" s="364"/>
+      <c r="I37" s="364"/>
       <c r="J37" s="167"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -27576,8 +27731,8 @@
       <c r="E38" s="127" t="s">
         <v>952</v>
       </c>
-      <c r="H38" s="282"/>
-      <c r="I38" s="282"/>
+      <c r="H38" s="364"/>
+      <c r="I38" s="364"/>
       <c r="J38" s="167" t="s">
         <v>961</v>
       </c>
@@ -27595,8 +27750,8 @@
       <c r="E39" s="127" t="s">
         <v>952</v>
       </c>
-      <c r="H39" s="282"/>
-      <c r="I39" s="282"/>
+      <c r="H39" s="364"/>
+      <c r="I39" s="364"/>
       <c r="J39" s="167" t="s">
         <v>963</v>
       </c>
@@ -27614,8 +27769,8 @@
       <c r="E40" s="170" t="s">
         <v>945</v>
       </c>
-      <c r="H40" s="282"/>
-      <c r="I40" s="282"/>
+      <c r="H40" s="364"/>
+      <c r="I40" s="364"/>
       <c r="J40" s="167"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
@@ -27631,8 +27786,8 @@
       <c r="E41" s="170" t="s">
         <v>945</v>
       </c>
-      <c r="H41" s="282"/>
-      <c r="I41" s="282"/>
+      <c r="H41" s="364"/>
+      <c r="I41" s="364"/>
       <c r="J41" s="167" t="s">
         <v>964</v>
       </c>
@@ -27650,8 +27805,8 @@
       <c r="E42" s="170" t="s">
         <v>945</v>
       </c>
-      <c r="H42" s="282"/>
-      <c r="I42" s="282"/>
+      <c r="H42" s="364"/>
+      <c r="I42" s="364"/>
       <c r="J42" s="167"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
@@ -27667,8 +27822,8 @@
       <c r="E43" s="170" t="s">
         <v>945</v>
       </c>
-      <c r="H43" s="282"/>
-      <c r="I43" s="282"/>
+      <c r="H43" s="364"/>
+      <c r="I43" s="364"/>
       <c r="J43" s="167"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
@@ -27684,8 +27839,8 @@
       <c r="E44" s="170" t="s">
         <v>945</v>
       </c>
-      <c r="H44" s="282"/>
-      <c r="I44" s="282"/>
+      <c r="H44" s="364"/>
+      <c r="I44" s="364"/>
       <c r="J44" s="167" t="s">
         <v>968</v>
       </c>
@@ -27735,8 +27890,8 @@
       <c r="E47" s="127" t="s">
         <v>909</v>
       </c>
-      <c r="H47" s="284"/>
-      <c r="I47" s="285" t="s">
+      <c r="H47" s="366"/>
+      <c r="I47" s="367" t="s">
         <v>972</v>
       </c>
       <c r="J47" s="167" t="s">
@@ -27756,8 +27911,8 @@
       <c r="E48" s="170" t="s">
         <v>909</v>
       </c>
-      <c r="H48" s="284"/>
-      <c r="I48" s="284"/>
+      <c r="H48" s="366"/>
+      <c r="I48" s="366"/>
       <c r="J48" s="167" t="s">
         <v>975</v>
       </c>
@@ -32774,7 +32929,7 @@
       <c r="C415" s="127" t="s">
         <v>1127</v>
       </c>
-      <c r="D415" s="234" t="s">
+      <c r="D415" s="233" t="s">
         <v>1677</v>
       </c>
       <c r="E415" s="130" t="s">
@@ -32792,7 +32947,7 @@
       <c r="C416" s="170" t="s">
         <v>1127</v>
       </c>
-      <c r="D416" s="234" t="s">
+      <c r="D416" s="233" t="s">
         <v>1678</v>
       </c>
       <c r="E416" s="173" t="s">
@@ -32873,16 +33028,16 @@
   </sheetData>
   <autoFilter ref="E1:E429"/>
   <mergeCells count="10">
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="F7:F19"/>
+    <mergeCell ref="G7:G12"/>
+    <mergeCell ref="G13:G19"/>
     <mergeCell ref="H24:H30"/>
     <mergeCell ref="H35:H44"/>
     <mergeCell ref="I35:I44"/>
     <mergeCell ref="H47:H48"/>
     <mergeCell ref="I47:I48"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="F7:F19"/>
-    <mergeCell ref="G7:G12"/>
-    <mergeCell ref="G13:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -32904,7 +33059,7 @@
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="121" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="121" customWidth="1"/>
-    <col min="4" max="4" width="36" style="236" customWidth="1"/>
+    <col min="4" max="4" width="36" style="235" customWidth="1"/>
     <col min="5" max="5" width="58.28515625" style="121" customWidth="1"/>
     <col min="6" max="6" width="67.28515625" customWidth="1"/>
     <col min="7" max="7" width="52.7109375" style="171" customWidth="1"/>
@@ -32914,45 +33069,45 @@
     <row r="1" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="121"/>
       <c r="C1" s="121"/>
-      <c r="D1" s="236"/>
+      <c r="D1" s="235"/>
       <c r="E1" s="121"/>
     </row>
     <row r="2" spans="1:8" s="171" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="121"/>
       <c r="C2" s="121"/>
-      <c r="D2" s="236"/>
+      <c r="D2" s="235"/>
       <c r="E2" s="121"/>
     </row>
     <row r="3" spans="1:8" s="171" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="288"/>
-      <c r="B3" s="291" t="s">
+      <c r="A3" s="277"/>
+      <c r="B3" s="280" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C3" s="279"/>
+      <c r="D3" s="279"/>
+      <c r="E3" s="279"/>
+      <c r="F3" s="277"/>
+      <c r="G3" s="277"/>
+      <c r="H3" s="277"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="236" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="236" t="s">
         <v>1738</v>
-      </c>
-      <c r="C3" s="290"/>
-      <c r="D3" s="290"/>
-      <c r="E3" s="290"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="288"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="237" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="237" t="s">
-        <v>1739</v>
       </c>
       <c r="C4" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="235" t="s">
+      <c r="D4" s="234" t="s">
         <v>1681</v>
       </c>
       <c r="E4" s="126" t="s">
         <v>1682</v>
       </c>
       <c r="F4" s="126" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="G4" s="126" t="s">
         <v>1683</v>
@@ -32962,29 +33117,29 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="238"/>
+      <c r="A5" s="237"/>
       <c r="B5" s="27" t="s">
         <v>889</v>
       </c>
       <c r="C5" s="27"/>
-      <c r="D5" s="239" t="s">
+      <c r="D5" s="238" t="s">
         <v>890</v>
       </c>
       <c r="E5" s="47" t="s">
         <v>891</v>
       </c>
-      <c r="F5" s="240" t="s">
+      <c r="F5" s="239" t="s">
         <v>1680</v>
       </c>
-      <c r="G5" s="241"/>
-      <c r="H5" s="238"/>
+      <c r="G5" s="240"/>
+      <c r="H5" s="237"/>
     </row>
     <row r="6" spans="1:8" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="238"/>
+      <c r="A6" s="237"/>
       <c r="B6" s="27" t="s">
         <v>889</v>
       </c>
-      <c r="C6" s="242">
+      <c r="C6" s="241">
         <v>3170</v>
       </c>
       <c r="D6" s="47" t="s">
@@ -32993,18 +33148,18 @@
       <c r="E6" s="14" t="s">
         <v>1228</v>
       </c>
-      <c r="F6" s="243" t="s">
+      <c r="F6" s="242" t="s">
         <v>1685</v>
       </c>
-      <c r="G6" s="244" t="s">
+      <c r="G6" s="243" t="s">
         <v>1684</v>
       </c>
-      <c r="H6" s="244" t="s">
+      <c r="H6" s="243" t="s">
         <v>1229</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="238"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="27" t="s">
         <v>889</v>
       </c>
@@ -33012,119 +33167,119 @@
       <c r="D7" s="14" t="s">
         <v>892</v>
       </c>
-      <c r="E7" s="245"/>
-      <c r="F7" s="246" t="s">
+      <c r="E7" s="244"/>
+      <c r="F7" s="245" t="s">
         <v>1231</v>
       </c>
-      <c r="G7" s="238"/>
-      <c r="H7" s="238"/>
+      <c r="G7" s="237"/>
+      <c r="H7" s="237"/>
     </row>
     <row r="8" spans="1:8" ht="240" x14ac:dyDescent="0.25">
-      <c r="A8" s="238"/>
-      <c r="B8" s="247" t="s">
+      <c r="A8" s="237"/>
+      <c r="B8" s="246" t="s">
         <v>893</v>
       </c>
-      <c r="C8" s="247"/>
+      <c r="C8" s="246"/>
       <c r="D8" s="14" t="s">
         <v>1232</v>
       </c>
       <c r="E8" s="47" t="s">
         <v>894</v>
       </c>
-      <c r="F8" s="248" t="s">
+      <c r="F8" s="247" t="s">
         <v>1689</v>
       </c>
-      <c r="G8" s="249" t="s">
+      <c r="G8" s="248" t="s">
         <v>1233</v>
       </c>
-      <c r="H8" s="238"/>
+      <c r="H8" s="237"/>
     </row>
     <row r="9" spans="1:8" ht="200.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="238"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="47" t="s">
         <v>895</v>
       </c>
       <c r="C9" s="47"/>
-      <c r="D9" s="250" t="s">
+      <c r="D9" s="249" t="s">
         <v>1690</v>
       </c>
-      <c r="E9" s="251" t="s">
+      <c r="E9" s="250" t="s">
         <v>1691</v>
       </c>
-      <c r="F9" s="248" t="s">
+      <c r="F9" s="247" t="s">
         <v>1692</v>
       </c>
-      <c r="G9" s="252"/>
-      <c r="H9" s="238"/>
-    </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="238"/>
+      <c r="G9" s="251"/>
+      <c r="H9" s="237"/>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="237"/>
       <c r="B10" s="47" t="s">
         <v>896</v>
       </c>
       <c r="C10" s="47"/>
-      <c r="D10" s="253" t="s">
+      <c r="D10" s="252" t="s">
         <v>897</v>
       </c>
-      <c r="E10" s="254" t="s">
+      <c r="E10" s="253" t="s">
         <v>1688</v>
       </c>
-      <c r="F10" s="240" t="s">
+      <c r="F10" s="239" t="s">
         <v>1687</v>
       </c>
-      <c r="G10" s="241"/>
-      <c r="H10" s="255"/>
+      <c r="G10" s="240"/>
+      <c r="H10" s="254"/>
     </row>
     <row r="11" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="219"/>
-      <c r="B11" s="292"/>
-      <c r="C11" s="292"/>
-      <c r="D11" s="293"/>
-      <c r="E11" s="294"/>
-      <c r="F11" s="295"/>
-      <c r="G11" s="296"/>
-      <c r="H11" s="297"/>
+      <c r="B11" s="281"/>
+      <c r="C11" s="281"/>
+      <c r="D11" s="282"/>
+      <c r="E11" s="283"/>
+      <c r="F11" s="284"/>
+      <c r="G11" s="285"/>
+      <c r="H11" s="286"/>
     </row>
     <row r="12" spans="1:8" s="171" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="219"/>
-      <c r="B12" s="292"/>
-      <c r="C12" s="292"/>
-      <c r="D12" s="293"/>
-      <c r="E12" s="294"/>
-      <c r="F12" s="295"/>
-      <c r="G12" s="296"/>
-      <c r="H12" s="297"/>
+      <c r="B12" s="281"/>
+      <c r="C12" s="281"/>
+      <c r="D12" s="282"/>
+      <c r="E12" s="283"/>
+      <c r="F12" s="284"/>
+      <c r="G12" s="285"/>
+      <c r="H12" s="286"/>
     </row>
     <row r="13" spans="1:8" s="171" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="288"/>
-      <c r="B13" s="291" t="s">
-        <v>1741</v>
-      </c>
-      <c r="C13" s="290"/>
-      <c r="D13" s="290"/>
-      <c r="E13" s="290"/>
-      <c r="F13" s="288"/>
-      <c r="G13" s="288"/>
-      <c r="H13" s="288"/>
+      <c r="A13" s="277"/>
+      <c r="B13" s="280" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C13" s="279"/>
+      <c r="D13" s="279"/>
+      <c r="E13" s="279"/>
+      <c r="F13" s="277"/>
+      <c r="G13" s="277"/>
+      <c r="H13" s="277"/>
     </row>
     <row r="14" spans="1:8" s="171" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="237" t="s">
+      <c r="A14" s="236" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="237" t="s">
+      <c r="B14" s="236" t="s">
         <v>888</v>
       </c>
       <c r="C14" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="235" t="s">
+      <c r="D14" s="234" t="s">
         <v>1681</v>
       </c>
       <c r="E14" s="126" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="F14" s="126" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="G14" s="126" t="s">
         <v>1683</v>
@@ -33134,200 +33289,200 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="331" t="s">
-        <v>1787</v>
+      <c r="B16" s="320" t="s">
+        <v>1786</v>
       </c>
       <c r="C16" s="121"/>
-      <c r="D16" s="236"/>
+      <c r="D16" s="235"/>
       <c r="E16" s="121"/>
     </row>
     <row r="17" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="171" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="C17" s="121"/>
       <c r="D17" s="171" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="E17" s="121"/>
     </row>
     <row r="18" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="329" t="s">
-        <v>1789</v>
+      <c r="B18" s="318" t="s">
+        <v>1788</v>
       </c>
       <c r="C18" s="121"/>
       <c r="D18" s="121" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="E18" s="121" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="F18" s="171" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="329" t="s">
-        <v>1791</v>
+      <c r="B19" s="318" t="s">
+        <v>1790</v>
       </c>
       <c r="C19" s="121"/>
-      <c r="D19" s="236"/>
+      <c r="D19" s="235"/>
       <c r="E19" s="121" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="F19" s="171" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="20" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="121"/>
       <c r="C20" s="121"/>
-      <c r="D20" s="236"/>
+      <c r="D20" s="235"/>
       <c r="E20" s="121"/>
       <c r="F20" s="171" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="21" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="121"/>
       <c r="C21" s="121"/>
-      <c r="D21" s="236"/>
+      <c r="D21" s="235"/>
       <c r="E21" s="121"/>
       <c r="F21" s="171" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="22" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="121"/>
       <c r="C22" s="121"/>
-      <c r="D22" s="236"/>
+      <c r="D22" s="235"/>
       <c r="F22" s="171" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="23" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="121"/>
       <c r="C23" s="121"/>
-      <c r="D23" s="236"/>
+      <c r="D23" s="235"/>
       <c r="E23" s="121"/>
       <c r="F23" s="171" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="24" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="121"/>
       <c r="C24" s="121"/>
-      <c r="D24" s="236"/>
+      <c r="D24" s="235"/>
       <c r="E24" s="121"/>
       <c r="F24" s="171" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="321" t="s">
         <v>1800</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="332" t="s">
-        <v>1801</v>
-      </c>
       <c r="C25" s="121"/>
-      <c r="D25" s="236"/>
-      <c r="E25" s="330" t="s">
-        <v>1810</v>
+      <c r="D25" s="235"/>
+      <c r="E25" s="319" t="s">
+        <v>1809</v>
       </c>
     </row>
     <row r="26" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="171" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="C26" s="121"/>
       <c r="D26" s="171" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="E26" s="121"/>
     </row>
     <row r="27" spans="2:6" s="171" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="329" t="s">
-        <v>1789</v>
+      <c r="B27" s="318" t="s">
+        <v>1788</v>
       </c>
       <c r="C27" s="121"/>
       <c r="D27" s="121" t="s">
-        <v>1788</v>
-      </c>
-      <c r="E27" s="236" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E27" s="235" t="s">
+        <v>1803</v>
+      </c>
+      <c r="F27" s="287" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="318" t="s">
+        <v>1801</v>
+      </c>
+      <c r="E28" s="121" t="s">
         <v>1804</v>
       </c>
-      <c r="F27" s="298" t="s">
+      <c r="F28" s="287" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" s="171" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="318"/>
+      <c r="C29" s="121"/>
+      <c r="D29" s="235"/>
+      <c r="E29" s="121" t="s">
         <v>1806</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="329" t="s">
-        <v>1802</v>
-      </c>
-      <c r="E28" s="121" t="s">
-        <v>1805</v>
-      </c>
-      <c r="F28" s="298" t="s">
-        <v>1809</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" s="171" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="329"/>
-      <c r="C29" s="121"/>
-      <c r="D29" s="236"/>
-      <c r="E29" s="121" t="s">
+      <c r="F29" s="287" t="s">
         <v>1807</v>
       </c>
-      <c r="F29" s="298" t="s">
-        <v>1808</v>
-      </c>
     </row>
     <row r="30" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="329"/>
+      <c r="B30" s="318"/>
       <c r="C30" s="121"/>
-      <c r="D30" s="236"/>
+      <c r="D30" s="235"/>
       <c r="E30" s="121"/>
     </row>
     <row r="31" spans="2:6" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="329"/>
+      <c r="B31" s="318"/>
       <c r="C31" s="121"/>
-      <c r="D31" s="236"/>
+      <c r="D31" s="235"/>
       <c r="E31" s="121"/>
     </row>
     <row r="32" spans="2:6" s="171" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="329"/>
+      <c r="B32" s="318"/>
       <c r="C32" s="121"/>
-      <c r="D32" s="236"/>
+      <c r="D32" s="235"/>
       <c r="E32" s="121"/>
     </row>
     <row r="33" spans="1:8" s="171" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="288"/>
-      <c r="B33" s="291" t="s">
-        <v>1743</v>
-      </c>
-      <c r="C33" s="290"/>
-      <c r="D33" s="290"/>
-      <c r="E33" s="290"/>
-      <c r="F33" s="288"/>
-      <c r="G33" s="288"/>
-      <c r="H33" s="288"/>
+      <c r="A33" s="277"/>
+      <c r="B33" s="280" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C33" s="279"/>
+      <c r="D33" s="279"/>
+      <c r="E33" s="279"/>
+      <c r="F33" s="277"/>
+      <c r="G33" s="277"/>
+      <c r="H33" s="277"/>
     </row>
     <row r="34" spans="1:8" s="171" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="237" t="s">
+      <c r="A34" s="236" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="237" t="s">
+      <c r="B34" s="236" t="s">
         <v>888</v>
       </c>
       <c r="C34" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="235" t="s">
+      <c r="D34" s="234" t="s">
         <v>1681</v>
       </c>
       <c r="E34" s="126" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="F34" s="126" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="G34" s="126" t="s">
         <v>1683</v>
@@ -33337,38 +33492,38 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B36" s="332" t="s">
+      <c r="B36" s="321" t="s">
+        <v>1810</v>
+      </c>
+      <c r="E36" s="121" t="s">
+        <v>1813</v>
+      </c>
+      <c r="F36" s="287" t="s">
         <v>1811</v>
-      </c>
-      <c r="E36" s="121" t="s">
-        <v>1814</v>
-      </c>
-      <c r="F36" s="298" t="s">
-        <v>1812</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B37" s="171"/>
       <c r="D37" s="171"/>
       <c r="E37" s="121" t="s">
+        <v>1814</v>
+      </c>
+      <c r="F37" s="287" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B38" s="318"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="318" t="s">
         <v>1815</v>
       </c>
-      <c r="F37" s="298" t="s">
-        <v>1813</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B38" s="329"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="329" t="s">
+      <c r="F38" s="287" t="s">
         <v>1816</v>
       </c>
-      <c r="F38" s="298" t="s">
-        <v>1817</v>
-      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="329"/>
+      <c r="B39" s="318"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
@@ -33378,309 +33533,345 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="6" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="6" width="24.140625" customWidth="1"/>
     <col min="7" max="8" width="24.140625" style="171" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="289" t="s">
+      <c r="A1" s="278" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="289" t="s">
+      <c r="B1" s="278" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C1" s="392"/>
+      <c r="D1" s="390" t="s">
         <v>1778</v>
       </c>
-      <c r="C1" s="289"/>
-      <c r="D1" s="171" t="s">
-        <v>1779</v>
-      </c>
+      <c r="E1" s="390"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="241"/>
-      <c r="B2" s="241" t="s">
+      <c r="A2" s="240"/>
+      <c r="B2" s="240" t="s">
         <v>1730</v>
       </c>
-      <c r="C2" s="241" t="s">
+      <c r="C2" s="240" t="s">
         <v>1731</v>
       </c>
-      <c r="D2" s="238" t="s">
+      <c r="D2" s="390" t="s">
         <v>1683</v>
       </c>
+      <c r="E2" s="390"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="238"/>
-      <c r="B3" s="238" t="s">
+      <c r="A3" s="237"/>
+      <c r="B3" s="237" t="s">
         <v>1727</v>
       </c>
-      <c r="C3" s="238" t="s">
+      <c r="C3" s="237" t="s">
         <v>325</v>
       </c>
-      <c r="D3" s="238" t="s">
+      <c r="D3" s="390" t="s">
         <v>1735</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="238"/>
-      <c r="B4" s="238" t="s">
+      <c r="E3" s="390"/>
+    </row>
+    <row r="4" spans="1:8" s="171" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="237"/>
+      <c r="B4" s="201" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C4" s="245" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D4" s="394" t="s">
+        <v>1847</v>
+      </c>
+      <c r="E4" s="394"/>
+      <c r="F4" s="393" t="s">
+        <v>1848</v>
+      </c>
+      <c r="G4" s="395" t="s">
+        <v>1850</v>
+      </c>
+      <c r="H4" s="395"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="237"/>
+      <c r="B5" s="237" t="s">
         <v>1728</v>
       </c>
-      <c r="C4" s="238" t="s">
+      <c r="C5" s="237" t="s">
         <v>325</v>
       </c>
-      <c r="D4" s="238" t="s">
+      <c r="D5" s="391" t="s">
         <v>1736</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="238"/>
-      <c r="B5" s="238" t="s">
+      <c r="E5" s="391"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="237"/>
+      <c r="B6" s="240" t="s">
         <v>879</v>
       </c>
-      <c r="C5" s="238" t="s">
-        <v>325</v>
-      </c>
-      <c r="D5" s="238" t="s">
-        <v>1737</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="241"/>
-      <c r="B6" s="241" t="s">
+      <c r="C6" s="240" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D6" s="390"/>
+      <c r="E6" s="390"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="240"/>
+      <c r="B7" s="240" t="s">
         <v>1729</v>
       </c>
-      <c r="C6" s="241" t="s">
+      <c r="C7" s="240" t="s">
         <v>1732</v>
       </c>
-      <c r="D6" s="238"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="241"/>
-      <c r="B7" s="241" t="s">
+      <c r="D7" s="390"/>
+      <c r="E7" s="390"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="240"/>
+      <c r="B8" s="240" t="s">
         <v>1733</v>
       </c>
-      <c r="C7" s="241" t="s">
+      <c r="C8" s="240" t="s">
         <v>1734</v>
       </c>
-      <c r="D7" s="238"/>
-    </row>
-    <row r="8" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="296"/>
-      <c r="B8" s="296"/>
-      <c r="C8" s="296"/>
-      <c r="D8" s="219"/>
+      <c r="D8" s="391"/>
+      <c r="E8" s="391"/>
     </row>
     <row r="9" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="296"/>
-      <c r="B9" s="296"/>
-      <c r="C9" s="296"/>
+      <c r="A9" s="285"/>
+      <c r="B9" s="285"/>
+      <c r="C9" s="285"/>
       <c r="D9" s="219"/>
     </row>
-    <row r="10" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="180" t="s">
+    <row r="10" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="285"/>
+      <c r="B10" s="285"/>
+      <c r="C10" s="285"/>
+      <c r="D10" s="219"/>
+    </row>
+    <row r="11" spans="1:8" s="171" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="180" t="s">
         <v>1676</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="221" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="221" t="s">
         <v>1647</v>
       </c>
-      <c r="C12" s="273" t="s">
+      <c r="C13" s="272" t="s">
         <v>1716</v>
       </c>
-      <c r="D12" s="275" t="s">
+      <c r="D13" s="274" t="s">
         <v>1721</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="222" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="222" t="s">
         <v>1648</v>
       </c>
-      <c r="C13" s="274" t="s">
+      <c r="C14" s="273" t="s">
         <v>1717</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="171" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="171" t="s">
         <v>1714</v>
       </c>
-      <c r="C14" s="171" t="s">
+      <c r="C15" s="171" t="s">
         <v>1715</v>
       </c>
-      <c r="H14" s="275" t="s">
+      <c r="H15" s="274" t="s">
         <v>1720</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="180" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="180" t="s">
         <v>1646</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="118" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="220" t="s">
+    <row r="20" spans="1:8" s="118" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="220" t="s">
         <v>1649</v>
       </c>
-      <c r="C19" s="226" t="s">
+      <c r="C20" s="226" t="s">
         <v>1651</v>
       </c>
-      <c r="D19" s="226" t="s">
+      <c r="D20" s="226" t="s">
         <v>1652</v>
       </c>
-      <c r="E19" s="286" t="s">
+      <c r="E20" s="371" t="s">
         <v>569</v>
       </c>
-      <c r="F19" s="287"/>
-      <c r="G19" s="226" t="s">
+      <c r="F20" s="372"/>
+      <c r="G20" s="226" t="s">
         <v>1659</v>
       </c>
-      <c r="H19" s="226" t="s">
+      <c r="H20" s="226" t="s">
         <v>1660</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="219" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="223" t="s">
+    <row r="21" spans="1:8" s="219" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="223" t="s">
         <v>1650</v>
       </c>
-      <c r="C20" s="224" t="s">
+      <c r="C21" s="224" t="s">
         <v>851</v>
       </c>
-      <c r="D20" s="224" t="s">
+      <c r="D21" s="224" t="s">
         <v>856</v>
       </c>
-      <c r="E20" s="225" t="s">
+      <c r="E21" s="225" t="s">
         <v>853</v>
       </c>
-      <c r="F20" s="225" t="s">
+      <c r="F21" s="225" t="s">
         <v>855</v>
       </c>
-      <c r="G20" s="224" t="s">
+      <c r="G21" s="224" t="s">
         <v>1658</v>
       </c>
-      <c r="H20" s="224"/>
-    </row>
-    <row r="21" spans="1:8" s="219" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B21" s="220" t="s">
+      <c r="H21" s="224"/>
+    </row>
+    <row r="22" spans="1:8" s="219" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B22" s="220" t="s">
         <v>1653</v>
       </c>
-      <c r="C21" s="227" t="s">
+      <c r="C22" s="227" t="s">
         <v>1663</v>
       </c>
-      <c r="D21" s="227"/>
-      <c r="E21" s="227" t="s">
+      <c r="D22" s="227"/>
+      <c r="E22" s="227" t="s">
         <v>1661</v>
       </c>
-      <c r="F21" s="233" t="s">
+      <c r="F22" s="232" t="s">
         <v>1675</v>
       </c>
-      <c r="G21" s="227" t="s">
+      <c r="G22" s="227" t="s">
         <v>1664</v>
       </c>
-      <c r="H21" s="231" t="s">
+      <c r="H22" s="231" t="s">
         <v>1665</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="219" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="220" t="s">
-        <v>1654</v>
-      </c>
-      <c r="C22" s="227" t="s">
-        <v>1666</v>
-      </c>
-      <c r="D22" s="227"/>
-      <c r="E22" s="227"/>
-      <c r="F22" s="228"/>
-      <c r="G22" s="227"/>
-      <c r="H22" s="227" t="s">
-        <v>1667</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="219" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="220" t="s">
-        <v>1655</v>
-      </c>
-      <c r="C23" s="229" t="s">
-        <v>1668</v>
+        <v>1654</v>
+      </c>
+      <c r="C23" s="227" t="s">
+        <v>1666</v>
       </c>
       <c r="D23" s="227"/>
-      <c r="E23" s="172" t="s">
-        <v>1673</v>
-      </c>
-      <c r="F23" s="232" t="s">
-        <v>1674</v>
-      </c>
+      <c r="E23" s="227"/>
+      <c r="F23" s="228"/>
       <c r="G23" s="227"/>
       <c r="H23" s="227" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="219" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="220" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C24" s="267" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D24" s="267"/>
+      <c r="E24" s="388" t="s">
+        <v>1673</v>
+      </c>
+      <c r="F24" s="389" t="s">
+        <v>1674</v>
+      </c>
+      <c r="G24" s="229"/>
+      <c r="H24" s="267" t="s">
         <v>1669</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="219" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="220" t="s">
+    <row r="25" spans="1:8" s="219" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="220" t="s">
         <v>1656</v>
       </c>
-      <c r="C24" s="229"/>
-      <c r="D24" s="269" t="s">
+      <c r="C25" s="267"/>
+      <c r="D25" s="268" t="s">
         <v>1662</v>
       </c>
-      <c r="E24" s="270" t="s">
+      <c r="E25" s="269" t="s">
         <v>1723</v>
       </c>
-      <c r="F24" s="269"/>
-      <c r="G24" s="229"/>
-      <c r="H24" s="268" t="s">
+      <c r="F25" s="268"/>
+      <c r="G25" s="229"/>
+      <c r="H25" s="267" t="s">
         <v>1670</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="219" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B25" s="220" t="s">
+    <row r="26" spans="1:8" s="219" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="220" t="s">
         <v>1657</v>
       </c>
-      <c r="C25" s="230" t="s">
+      <c r="C26" s="230" t="s">
         <v>1672</v>
       </c>
-      <c r="D25" s="227"/>
-      <c r="E25" s="272" t="s">
+      <c r="D26" s="227"/>
+      <c r="E26" s="271" t="s">
         <v>1722</v>
       </c>
-      <c r="F25" s="272" t="s">
+      <c r="F26" s="271" t="s">
         <v>1713</v>
       </c>
-      <c r="G25" s="227"/>
-      <c r="H25" s="271" t="s">
+      <c r="G26" s="227"/>
+      <c r="H26" s="270" t="s">
         <v>1671</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="150" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="150" t="s">
         <v>1718</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="171" t="s">
         <v>1768</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="171" t="s">
-        <v>1769</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E19:F19"/>
+  <mergeCells count="10">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -33702,75 +33893,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="238"/>
-      <c r="D1" s="238" t="s">
-        <v>1781</v>
-      </c>
-      <c r="E1" s="238" t="s">
-        <v>1746</v>
-      </c>
-      <c r="F1" s="238" t="s">
+      <c r="C1" s="237"/>
+      <c r="D1" s="237" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E1" s="237" t="s">
         <v>1745</v>
       </c>
-      <c r="G1" s="238" t="s">
+      <c r="F1" s="237" t="s">
         <v>1744</v>
       </c>
+      <c r="G1" s="237" t="s">
+        <v>1743</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="238" t="s">
-        <v>1780</v>
-      </c>
-      <c r="D2" s="238">
+      <c r="C2" s="237" t="s">
+        <v>1779</v>
+      </c>
+      <c r="D2" s="237">
         <v>0</v>
       </c>
-      <c r="E2" s="238">
+      <c r="E2" s="237">
         <v>0</v>
       </c>
-      <c r="F2" s="238">
+      <c r="F2" s="237">
         <v>0</v>
       </c>
-      <c r="G2" s="238">
+      <c r="G2" s="237">
         <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:7" s="171" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="289" t="s">
+      <c r="A5" s="278" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="289" t="s">
+      <c r="B5" s="278" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C5" s="278"/>
+      <c r="D5" s="328" t="s">
         <v>1782</v>
       </c>
-      <c r="C5" s="289"/>
-      <c r="D5" s="339" t="s">
+    </row>
+    <row r="6" spans="1:7" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="240"/>
+      <c r="B6" s="240" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C6" s="240" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="240"/>
+      <c r="B7" s="317" t="s">
         <v>1783</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="241"/>
-      <c r="B6" s="241" t="s">
-        <v>1786</v>
-      </c>
-      <c r="C6" s="241" t="s">
-        <v>1731</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="241"/>
-      <c r="B7" s="328" t="s">
+      <c r="C7" s="317" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="237"/>
+      <c r="B8" s="240" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="240" t="s">
         <v>1784</v>
-      </c>
-      <c r="C7" s="328" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="238"/>
-      <c r="B8" s="241" t="s">
-        <v>288</v>
-      </c>
-      <c r="C8" s="241" t="s">
-        <v>1785</v>
       </c>
     </row>
   </sheetData>
@@ -33782,14 +33973,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="256" customWidth="1"/>
-    <col min="2" max="3" width="16.5703125" style="256" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="255" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" style="255" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="52.140625" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
@@ -33799,408 +33990,408 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="171" customFormat="1" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="262"/>
-      <c r="B1" s="340" t="s">
+      <c r="A1" s="261"/>
+      <c r="B1" s="329" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+    </row>
+    <row r="2" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="333" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C2" s="333" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D2" s="333" t="s">
+        <v>1829</v>
+      </c>
+      <c r="G2" s="255"/>
+    </row>
+    <row r="3" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="333" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C3" s="333" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D3" s="334" t="s">
+        <v>1830</v>
+      </c>
+      <c r="E3" s="335" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="333" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C4" s="334" t="s">
+        <v>1831</v>
+      </c>
+      <c r="D4" s="334" t="s">
+        <v>1830</v>
+      </c>
+      <c r="E4" s="335" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="333" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C5" s="333" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D5" s="334" t="s">
+        <v>1830</v>
+      </c>
+      <c r="E5" s="335" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="331" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="362" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="171" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="261"/>
+      <c r="B7" s="261" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C7" s="261" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D7" s="261" t="s">
+        <v>1835</v>
+      </c>
+      <c r="E7" s="261" t="s">
         <v>1819</v>
       </c>
-      <c r="C1" s="262"/>
-      <c r="D1" s="262"/>
-      <c r="E1" s="262"/>
-    </row>
-    <row r="2" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="356" t="s">
-        <v>1744</v>
-      </c>
-      <c r="C2" s="356" t="s">
-        <v>1829</v>
-      </c>
-      <c r="D2" s="356" t="s">
-        <v>1830</v>
-      </c>
-      <c r="G2" s="256"/>
-    </row>
-    <row r="3" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="356" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C3" s="356" t="s">
-        <v>1829</v>
-      </c>
-      <c r="D3" s="357" t="s">
-        <v>1831</v>
-      </c>
-      <c r="E3" s="361" t="s">
+      <c r="F7" s="336" t="s">
+        <v>1712</v>
+      </c>
+      <c r="G7" s="336" t="s">
+        <v>1701</v>
+      </c>
+      <c r="H7" s="336" t="s">
+        <v>1824</v>
+      </c>
+      <c r="I7" s="336" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="373" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C8" s="376" t="s">
         <v>1837</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="356" t="s">
-        <v>1746</v>
-      </c>
-      <c r="C4" s="357" t="s">
-        <v>1832</v>
-      </c>
-      <c r="D4" s="357" t="s">
-        <v>1831</v>
-      </c>
-      <c r="E4" s="361" t="s">
+      <c r="D8" s="379" t="s">
+        <v>1702</v>
+      </c>
+      <c r="E8" s="382" t="s">
+        <v>1826</v>
+      </c>
+      <c r="F8" s="337" t="s">
+        <v>1699</v>
+      </c>
+      <c r="G8" s="338" t="s">
+        <v>1704</v>
+      </c>
+      <c r="H8" s="339" t="s">
+        <v>1838</v>
+      </c>
+      <c r="I8" s="340" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="255"/>
+      <c r="B9" s="374"/>
+      <c r="C9" s="377"/>
+      <c r="D9" s="380"/>
+      <c r="E9" s="383"/>
+      <c r="F9" s="341" t="s">
+        <v>1699</v>
+      </c>
+      <c r="G9" s="342" t="s">
+        <v>266</v>
+      </c>
+      <c r="H9" s="343" t="s">
+        <v>1840</v>
+      </c>
+      <c r="I9" s="344" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="255"/>
+      <c r="B10" s="374"/>
+      <c r="C10" s="377"/>
+      <c r="D10" s="380"/>
+      <c r="E10" s="383"/>
+      <c r="F10" s="345" t="s">
+        <v>1699</v>
+      </c>
+      <c r="G10" s="346" t="s">
+        <v>1705</v>
+      </c>
+      <c r="H10" s="347" t="s">
+        <v>1823</v>
+      </c>
+      <c r="I10" s="348"/>
+    </row>
+    <row r="11" spans="1:9" s="171" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="255"/>
+      <c r="B11" s="375"/>
+      <c r="C11" s="378"/>
+      <c r="D11" s="381"/>
+      <c r="E11" s="384"/>
+      <c r="F11" s="349" t="s">
+        <v>1705</v>
+      </c>
+      <c r="G11" s="350" t="s">
+        <v>1822</v>
+      </c>
+      <c r="H11" s="351" t="s">
+        <v>1821</v>
+      </c>
+      <c r="I11" s="352" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="171" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A12" s="255"/>
+      <c r="B12" s="373" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C12" s="379" t="s">
         <v>1837</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="356" t="s">
-        <v>1747</v>
-      </c>
-      <c r="C5" s="356" t="s">
-        <v>1829</v>
-      </c>
-      <c r="D5" s="357" t="s">
-        <v>1831</v>
-      </c>
-      <c r="E5" s="361" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="342" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="388" t="s">
-        <v>1847</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="171" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="262"/>
-      <c r="B7" s="262" t="s">
-        <v>1834</v>
-      </c>
-      <c r="C7" s="262" t="s">
-        <v>1835</v>
-      </c>
-      <c r="D7" s="262" t="s">
-        <v>1836</v>
-      </c>
-      <c r="E7" s="262" t="s">
+      <c r="D12" s="379" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E12" s="385" t="s">
         <v>1820</v>
       </c>
-      <c r="F7" s="362" t="s">
-        <v>1712</v>
-      </c>
-      <c r="G7" s="362" t="s">
-        <v>1701</v>
-      </c>
-      <c r="H7" s="362" t="s">
-        <v>1825</v>
-      </c>
-      <c r="I7" s="362" t="s">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="343" t="s">
-        <v>1699</v>
-      </c>
-      <c r="C8" s="345" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D8" s="347" t="s">
-        <v>1702</v>
-      </c>
-      <c r="E8" s="358" t="s">
-        <v>1827</v>
-      </c>
-      <c r="F8" s="363" t="s">
-        <v>1699</v>
-      </c>
-      <c r="G8" s="364" t="s">
+      <c r="F12" s="353" t="s">
+        <v>1700</v>
+      </c>
+      <c r="G12" s="354" t="s">
         <v>1704</v>
       </c>
-      <c r="H8" s="365" t="s">
-        <v>1839</v>
-      </c>
-      <c r="I8" s="366" t="s">
-        <v>1840</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="256"/>
-      <c r="B9" s="344"/>
-      <c r="C9" s="346"/>
-      <c r="D9" s="348"/>
-      <c r="E9" s="359"/>
-      <c r="F9" s="367" t="s">
-        <v>1699</v>
-      </c>
-      <c r="G9" s="368" t="s">
+      <c r="H12" s="355" t="s">
+        <v>1841</v>
+      </c>
+      <c r="I12" s="356" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="255"/>
+      <c r="B13" s="374"/>
+      <c r="C13" s="380"/>
+      <c r="D13" s="380"/>
+      <c r="E13" s="386"/>
+      <c r="F13" s="341" t="s">
+        <v>1700</v>
+      </c>
+      <c r="G13" s="342" t="s">
         <v>266</v>
       </c>
-      <c r="H9" s="369" t="s">
-        <v>1841</v>
-      </c>
-      <c r="I9" s="370" t="s">
-        <v>1708</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="256"/>
-      <c r="B10" s="344"/>
-      <c r="C10" s="346"/>
-      <c r="D10" s="348"/>
-      <c r="E10" s="359"/>
-      <c r="F10" s="371" t="s">
-        <v>1699</v>
-      </c>
-      <c r="G10" s="372" t="s">
+      <c r="H13" s="343" t="s">
+        <v>1843</v>
+      </c>
+      <c r="I13" s="344" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="255"/>
+      <c r="B14" s="374"/>
+      <c r="C14" s="380"/>
+      <c r="D14" s="380"/>
+      <c r="E14" s="386"/>
+      <c r="F14" s="345" t="s">
+        <v>1700</v>
+      </c>
+      <c r="G14" s="346" t="s">
         <v>1705</v>
       </c>
-      <c r="H10" s="373" t="s">
-        <v>1824</v>
-      </c>
-      <c r="I10" s="374"/>
-    </row>
-    <row r="11" spans="1:9" s="171" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="256"/>
-      <c r="B11" s="351"/>
-      <c r="C11" s="352"/>
-      <c r="D11" s="353"/>
-      <c r="E11" s="360"/>
-      <c r="F11" s="375" t="s">
+      <c r="H14" s="347" t="s">
+        <v>1823</v>
+      </c>
+      <c r="I14" s="357"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="375"/>
+      <c r="C15" s="381"/>
+      <c r="D15" s="381"/>
+      <c r="E15" s="387"/>
+      <c r="F15" s="349" t="s">
         <v>1705</v>
       </c>
-      <c r="G11" s="376" t="s">
-        <v>1823</v>
-      </c>
-      <c r="H11" s="377" t="s">
-        <v>1822</v>
-      </c>
-      <c r="I11" s="378" t="s">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="171" customFormat="1" ht="48" x14ac:dyDescent="0.25">
-      <c r="A12" s="256"/>
-      <c r="B12" s="343" t="s">
-        <v>1700</v>
-      </c>
-      <c r="C12" s="347" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D12" s="347" t="s">
-        <v>1703</v>
-      </c>
-      <c r="E12" s="349" t="s">
-        <v>1821</v>
-      </c>
-      <c r="F12" s="379" t="s">
-        <v>1700</v>
-      </c>
-      <c r="G12" s="380" t="s">
-        <v>1704</v>
-      </c>
-      <c r="H12" s="381" t="s">
-        <v>1842</v>
-      </c>
-      <c r="I12" s="382" t="s">
-        <v>1843</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="256"/>
-      <c r="B13" s="344"/>
-      <c r="C13" s="348"/>
-      <c r="D13" s="348"/>
-      <c r="E13" s="350"/>
-      <c r="F13" s="367" t="s">
-        <v>1700</v>
-      </c>
-      <c r="G13" s="368" t="s">
+      <c r="G15" s="350" t="s">
         <v>266</v>
       </c>
-      <c r="H13" s="369" t="s">
+      <c r="H15" s="358" t="s">
         <v>1844</v>
       </c>
-      <c r="I13" s="370" t="s">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
-      <c r="B14" s="344"/>
-      <c r="C14" s="348"/>
-      <c r="D14" s="348"/>
-      <c r="E14" s="350"/>
-      <c r="F14" s="371" t="s">
-        <v>1700</v>
-      </c>
-      <c r="G14" s="372" t="s">
+      <c r="I15" s="352" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="171" customFormat="1" ht="49.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="255"/>
+      <c r="B16" s="258"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="330"/>
+      <c r="F16" s="359" t="s">
         <v>1705</v>
       </c>
-      <c r="H14" s="373" t="s">
-        <v>1824</v>
-      </c>
-      <c r="I14" s="383"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="351"/>
-      <c r="C15" s="353"/>
-      <c r="D15" s="353"/>
-      <c r="E15" s="354"/>
-      <c r="F15" s="375" t="s">
+      <c r="G16" s="360" t="s">
         <v>1705</v>
       </c>
-      <c r="G15" s="376" t="s">
-        <v>266</v>
-      </c>
-      <c r="H15" s="384" t="s">
+      <c r="H16" s="361" t="s">
         <v>1845</v>
       </c>
-      <c r="I15" s="378" t="s">
-        <v>1706</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="171" customFormat="1" ht="49.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="256"/>
-      <c r="B16" s="259"/>
-      <c r="C16" s="261"/>
-      <c r="D16" s="261"/>
-      <c r="E16" s="341"/>
-      <c r="F16" s="385" t="s">
-        <v>1705</v>
-      </c>
-      <c r="G16" s="386" t="s">
-        <v>1705</v>
-      </c>
-      <c r="H16" s="387" t="s">
-        <v>1846</v>
-      </c>
-      <c r="I16" s="378" t="s">
+      <c r="I16" s="352" t="s">
         <v>1710</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="256"/>
-      <c r="B17" s="259"/>
-      <c r="C17" s="261"/>
-      <c r="D17" s="261"/>
-      <c r="E17" s="341"/>
-      <c r="F17" s="259"/>
-      <c r="G17" s="259"/>
-      <c r="H17" s="341"/>
-      <c r="I17" s="355"/>
+      <c r="A17" s="255"/>
+      <c r="B17" s="258"/>
+      <c r="C17" s="260"/>
+      <c r="D17" s="260"/>
+      <c r="E17" s="330"/>
+      <c r="F17" s="258"/>
+      <c r="G17" s="258"/>
+      <c r="H17" s="330"/>
+      <c r="I17" s="332"/>
     </row>
     <row r="18" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="256"/>
-      <c r="B18" s="259"/>
-      <c r="C18" s="261"/>
-      <c r="D18" s="261"/>
-      <c r="E18" s="341"/>
-      <c r="F18" s="259"/>
-      <c r="G18" s="259"/>
-      <c r="H18" s="341"/>
-      <c r="I18" s="355"/>
+      <c r="A18" s="255"/>
+      <c r="B18" s="258"/>
+      <c r="C18" s="260"/>
+      <c r="D18" s="260"/>
+      <c r="E18" s="330"/>
+      <c r="F18" s="258"/>
+      <c r="G18" s="258"/>
+      <c r="H18" s="330"/>
+      <c r="I18" s="332"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:9" s="171" customFormat="1" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="262"/>
-      <c r="B20" s="340" t="s">
-        <v>1828</v>
-      </c>
-      <c r="C20" s="262"/>
-      <c r="D20" s="262"/>
-      <c r="E20" s="262"/>
-    </row>
-    <row r="21" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="356" t="s">
+      <c r="A20" s="261"/>
+      <c r="B20" s="329" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C20" s="261"/>
+      <c r="D20" s="261"/>
+      <c r="E20" s="261"/>
+    </row>
+    <row r="21" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="333" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C21" s="333" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="333" t="s">
         <v>1744</v>
       </c>
-      <c r="C21" s="356" t="s">
+      <c r="C22" s="334" t="s">
         <v>1830</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="356" t="s">
+      <c r="D22" s="335" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="333" t="s">
         <v>1745</v>
       </c>
-      <c r="C22" s="357" t="s">
-        <v>1831</v>
-      </c>
-      <c r="D22" s="361" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="356" t="s">
+      <c r="C23" s="334" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D23" s="335" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="331" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="333" t="s">
         <v>1746</v>
       </c>
-      <c r="C23" s="357" t="s">
-        <v>1831</v>
-      </c>
-      <c r="D23" s="361" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="342" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="356" t="s">
-        <v>1747</v>
-      </c>
-      <c r="C24" s="357" t="s">
-        <v>1831</v>
-      </c>
-      <c r="D24" s="361" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="342" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C24" s="334" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D24" s="335" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="331" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:9" s="171" customFormat="1" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="262"/>
-      <c r="B26" s="262" t="s">
-        <v>1833</v>
-      </c>
-      <c r="C26" s="262"/>
-      <c r="D26" s="262" t="s">
+      <c r="A26" s="261"/>
+      <c r="B26" s="261" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C26" s="261"/>
+      <c r="D26" s="261" t="s">
         <v>1696</v>
       </c>
-      <c r="E26" s="262" t="s">
+      <c r="E26" s="261" t="s">
         <v>1711</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="256"/>
-      <c r="B27" s="263">
+      <c r="A27" s="255"/>
+      <c r="B27" s="262">
         <v>1</v>
       </c>
-      <c r="C27" s="258"/>
-      <c r="D27" s="258" t="s">
+      <c r="C27" s="257"/>
+      <c r="D27" s="257" t="s">
         <v>1693</v>
       </c>
-      <c r="E27" s="264"/>
+      <c r="E27" s="263"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="265">
+      <c r="B28" s="264">
         <v>2</v>
       </c>
-      <c r="C28" s="261"/>
-      <c r="D28" s="261" t="s">
+      <c r="C28" s="260"/>
+      <c r="D28" s="260" t="s">
         <v>1694</v>
       </c>
-      <c r="E28" s="260"/>
+      <c r="E28" s="259"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="265">
+      <c r="B29" s="264">
         <v>3</v>
       </c>
-      <c r="C29" s="261"/>
-      <c r="D29" s="261" t="s">
+      <c r="C29" s="260"/>
+      <c r="D29" s="260" t="s">
         <v>1695</v>
       </c>
-      <c r="E29" s="260"/>
+      <c r="E29" s="259"/>
     </row>
     <row r="30" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="266" t="s">
+      <c r="B30" s="265" t="s">
         <v>1697</v>
       </c>
-      <c r="C30" s="257"/>
-      <c r="D30" s="257" t="s">
+      <c r="C30" s="256"/>
+      <c r="D30" s="256" t="s">
         <v>325</v>
       </c>
-      <c r="E30" s="267" t="s">
+      <c r="E30" s="266" t="s">
         <v>1698</v>
       </c>
     </row>

</xml_diff>